<commit_message>
add stardust and party order doc
</commit_message>
<xml_diff>
--- a/LODEdit/Additional/memory_map.xlsx
+++ b/LODEdit/Additional/memory_map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brett\Documents\memcardrex-plugins-LODEdit\LODEdit\Additional\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A87F61A5-09A5-4CCA-8158-C4328D7D595C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBCB2B83-87EF-42E2-8D01-7EB38572046A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
   <si>
     <t>Address</t>
   </si>
@@ -164,6 +164,9 @@
   <si>
     <t>Zychronix, greenbrettmichael</t>
   </si>
+  <si>
+    <t>Stardust</t>
+  </si>
 </sst>
 </file>
 
@@ -215,7 +218,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -288,6 +291,12 @@
         <bgColor rgb="FFFF00FF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -301,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -356,36 +365,27 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -393,11 +393,25 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -618,9 +632,9 @@
   </sheetPr>
   <dimension ref="A1:T520"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P42" sqref="P42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -698,26 +712,26 @@
         <f t="shared" ref="B2:B520" si="0">DEC2HEX(A2)</f>
         <v>10</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="33" t="s">
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="24"/>
       <c r="S2" s="6"/>
       <c r="T2" t="s">
         <v>43</v>
@@ -731,26 +745,26 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="27" t="s">
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="21"/>
-      <c r="R3" s="21"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24"/>
+      <c r="Q3" s="24"/>
+      <c r="R3" s="24"/>
       <c r="S3" s="6"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
@@ -903,10 +917,10 @@
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
       <c r="N9" s="10"/>
-      <c r="O9" s="35"/>
-      <c r="P9" s="34"/>
-      <c r="Q9" s="34"/>
-      <c r="R9" s="34"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="21"/>
+      <c r="R9" s="21"/>
       <c r="S9" s="13"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
@@ -1523,18 +1537,18 @@
       <c r="H33" s="10"/>
       <c r="I33" s="10"/>
       <c r="J33" s="10"/>
-      <c r="K33" s="27" t="s">
+      <c r="K33" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="L33" s="21"/>
-      <c r="M33" s="21"/>
-      <c r="N33" s="21"/>
-      <c r="O33" s="23" t="s">
+      <c r="L33" s="24"/>
+      <c r="M33" s="24"/>
+      <c r="N33" s="24"/>
+      <c r="O33" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="P33" s="21"/>
-      <c r="Q33" s="21"/>
-      <c r="R33" s="21"/>
+      <c r="P33" s="24"/>
+      <c r="Q33" s="24"/>
+      <c r="R33" s="24"/>
       <c r="S33" s="12"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.2">
@@ -1545,28 +1559,28 @@
         <f t="shared" si="0"/>
         <v>210</v>
       </c>
-      <c r="C34" s="25" t="s">
+      <c r="C34" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="26" t="s">
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="H34" s="21"/>
+      <c r="H34" s="24"/>
       <c r="I34" s="10"/>
       <c r="J34" s="10"/>
       <c r="K34" s="10"/>
       <c r="L34" s="10"/>
       <c r="M34" s="10"/>
       <c r="N34" s="10"/>
-      <c r="O34" s="20" t="s">
+      <c r="O34" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="P34" s="21"/>
-      <c r="Q34" s="21"/>
-      <c r="R34" s="21"/>
+      <c r="P34" s="24"/>
+      <c r="Q34" s="24"/>
+      <c r="R34" s="24"/>
       <c r="S34" s="16" t="s">
         <v>16</v>
       </c>
@@ -1579,26 +1593,28 @@
         <f t="shared" si="0"/>
         <v>220</v>
       </c>
-      <c r="C35" s="22" t="s">
+      <c r="C35" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
       <c r="G35" s="17" t="s">
         <v>18</v>
       </c>
       <c r="H35" s="10"/>
       <c r="I35" s="10"/>
       <c r="J35" s="10"/>
-      <c r="K35" s="10"/>
-      <c r="L35" s="10"/>
-      <c r="M35" s="10"/>
-      <c r="N35" s="10"/>
-      <c r="O35" s="24"/>
-      <c r="P35" s="21"/>
-      <c r="Q35" s="21"/>
-      <c r="R35" s="21"/>
+      <c r="K35" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="L35" s="37"/>
+      <c r="M35" s="37"/>
+      <c r="N35" s="37"/>
+      <c r="O35" s="38"/>
+      <c r="P35" s="20"/>
+      <c r="Q35" s="20"/>
+      <c r="R35" s="20"/>
       <c r="S35" s="16" t="s">
         <v>19</v>
       </c>
@@ -1957,14 +1973,18 @@
       <c r="H49" s="10"/>
       <c r="I49" s="10"/>
       <c r="J49" s="10"/>
-      <c r="K49" s="10"/>
-      <c r="L49" s="10"/>
-      <c r="M49" s="10"/>
-      <c r="N49" s="10"/>
-      <c r="O49" s="10"/>
-      <c r="P49" s="10"/>
-      <c r="Q49" s="10"/>
-      <c r="R49" s="10"/>
+      <c r="K49" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="L49" s="24"/>
+      <c r="M49" s="24"/>
+      <c r="N49" s="24"/>
+      <c r="O49" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="P49" s="24"/>
+      <c r="Q49" s="24"/>
+      <c r="R49" s="24"/>
       <c r="S49" s="12"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.2">
@@ -1975,24 +1995,28 @@
         <f t="shared" si="0"/>
         <v>310</v>
       </c>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="10"/>
-      <c r="G50" s="20" t="s">
+      <c r="C50" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50" s="24"/>
+      <c r="E50" s="24"/>
+      <c r="F50" s="24"/>
+      <c r="G50" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="H50" s="21"/>
-      <c r="I50" s="21"/>
-      <c r="J50" s="21"/>
+      <c r="H50" s="24"/>
+      <c r="I50" s="24"/>
+      <c r="J50" s="24"/>
       <c r="K50" s="10"/>
       <c r="L50" s="10"/>
       <c r="M50" s="10"/>
       <c r="N50" s="10"/>
-      <c r="O50" s="10"/>
-      <c r="P50" s="10"/>
-      <c r="Q50" s="10"/>
-      <c r="R50" s="10"/>
+      <c r="O50" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="P50" s="37"/>
+      <c r="Q50" s="37"/>
+      <c r="R50" s="37"/>
       <c r="S50" s="12"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.2">
@@ -2003,12 +2027,12 @@
         <f t="shared" si="0"/>
         <v>320</v>
       </c>
-      <c r="C51" s="22" t="s">
+      <c r="C51" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="D51" s="21"/>
-      <c r="E51" s="21"/>
-      <c r="F51" s="21"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="24"/>
       <c r="G51" s="5" t="s">
         <v>20</v>
       </c>
@@ -2039,10 +2063,10 @@
       <c r="D52" s="10"/>
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
-      <c r="G52" s="23" t="s">
+      <c r="G52" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="H52" s="21"/>
+      <c r="H52" s="24"/>
       <c r="I52" s="10"/>
       <c r="J52" s="10"/>
       <c r="L52" s="10"/>
@@ -2552,14 +2576,14 @@
         <v>27</v>
       </c>
       <c r="J71" s="10"/>
-      <c r="K71" s="22"/>
-      <c r="L71" s="21"/>
-      <c r="M71" s="21"/>
-      <c r="N71" s="21"/>
-      <c r="O71" s="21"/>
-      <c r="P71" s="21"/>
-      <c r="Q71" s="21"/>
-      <c r="R71" s="21"/>
+      <c r="K71" s="29"/>
+      <c r="L71" s="24"/>
+      <c r="M71" s="24"/>
+      <c r="N71" s="24"/>
+      <c r="O71" s="24"/>
+      <c r="P71" s="24"/>
+      <c r="Q71" s="24"/>
+      <c r="R71" s="24"/>
       <c r="S71" s="16" t="s">
         <v>28</v>
       </c>
@@ -2572,24 +2596,24 @@
         <f t="shared" si="0"/>
         <v>470</v>
       </c>
-      <c r="C72" s="30" t="s">
+      <c r="C72" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D72" s="21"/>
-      <c r="E72" s="21"/>
-      <c r="F72" s="21"/>
-      <c r="G72" s="21"/>
-      <c r="H72" s="21"/>
-      <c r="I72" s="21"/>
-      <c r="J72" s="21"/>
-      <c r="K72" s="21"/>
-      <c r="L72" s="21"/>
-      <c r="M72" s="21"/>
-      <c r="N72" s="21"/>
-      <c r="O72" s="21"/>
-      <c r="P72" s="21"/>
-      <c r="Q72" s="21"/>
-      <c r="R72" s="21"/>
+      <c r="D72" s="24"/>
+      <c r="E72" s="24"/>
+      <c r="F72" s="24"/>
+      <c r="G72" s="24"/>
+      <c r="H72" s="24"/>
+      <c r="I72" s="24"/>
+      <c r="J72" s="24"/>
+      <c r="K72" s="24"/>
+      <c r="L72" s="24"/>
+      <c r="M72" s="24"/>
+      <c r="N72" s="24"/>
+      <c r="O72" s="24"/>
+      <c r="P72" s="24"/>
+      <c r="Q72" s="24"/>
+      <c r="R72" s="24"/>
       <c r="S72" s="12"/>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.2">
@@ -2600,22 +2624,22 @@
         <f t="shared" si="0"/>
         <v>480</v>
       </c>
-      <c r="C73" s="21"/>
-      <c r="D73" s="21"/>
-      <c r="E73" s="21"/>
-      <c r="F73" s="21"/>
-      <c r="G73" s="21"/>
-      <c r="H73" s="21"/>
-      <c r="I73" s="21"/>
-      <c r="J73" s="21"/>
-      <c r="K73" s="21"/>
-      <c r="L73" s="21"/>
-      <c r="M73" s="21"/>
-      <c r="N73" s="21"/>
-      <c r="O73" s="21"/>
-      <c r="P73" s="21"/>
-      <c r="Q73" s="21"/>
-      <c r="R73" s="21"/>
+      <c r="C73" s="24"/>
+      <c r="D73" s="24"/>
+      <c r="E73" s="24"/>
+      <c r="F73" s="24"/>
+      <c r="G73" s="24"/>
+      <c r="H73" s="24"/>
+      <c r="I73" s="24"/>
+      <c r="J73" s="24"/>
+      <c r="K73" s="24"/>
+      <c r="L73" s="24"/>
+      <c r="M73" s="24"/>
+      <c r="N73" s="24"/>
+      <c r="O73" s="24"/>
+      <c r="P73" s="24"/>
+      <c r="Q73" s="24"/>
+      <c r="R73" s="24"/>
       <c r="S73" s="12"/>
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.2">
@@ -2626,22 +2650,22 @@
         <f t="shared" si="0"/>
         <v>490</v>
       </c>
-      <c r="C74" s="21"/>
-      <c r="D74" s="21"/>
-      <c r="E74" s="21"/>
-      <c r="F74" s="21"/>
-      <c r="G74" s="21"/>
-      <c r="H74" s="21"/>
-      <c r="I74" s="21"/>
-      <c r="J74" s="21"/>
-      <c r="K74" s="21"/>
-      <c r="L74" s="21"/>
-      <c r="M74" s="21"/>
-      <c r="N74" s="21"/>
-      <c r="O74" s="21"/>
-      <c r="P74" s="21"/>
-      <c r="Q74" s="21"/>
-      <c r="R74" s="21"/>
+      <c r="C74" s="24"/>
+      <c r="D74" s="24"/>
+      <c r="E74" s="24"/>
+      <c r="F74" s="24"/>
+      <c r="G74" s="24"/>
+      <c r="H74" s="24"/>
+      <c r="I74" s="24"/>
+      <c r="J74" s="24"/>
+      <c r="K74" s="24"/>
+      <c r="L74" s="24"/>
+      <c r="M74" s="24"/>
+      <c r="N74" s="24"/>
+      <c r="O74" s="24"/>
+      <c r="P74" s="24"/>
+      <c r="Q74" s="24"/>
+      <c r="R74" s="24"/>
       <c r="S74" s="12"/>
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.2">
@@ -2652,22 +2676,22 @@
         <f t="shared" si="0"/>
         <v>4A0</v>
       </c>
-      <c r="C75" s="21"/>
-      <c r="D75" s="21"/>
-      <c r="E75" s="21"/>
-      <c r="F75" s="21"/>
-      <c r="G75" s="21"/>
-      <c r="H75" s="21"/>
-      <c r="I75" s="21"/>
-      <c r="J75" s="21"/>
-      <c r="K75" s="21"/>
-      <c r="L75" s="21"/>
-      <c r="M75" s="21"/>
-      <c r="N75" s="21"/>
-      <c r="O75" s="21"/>
-      <c r="P75" s="21"/>
-      <c r="Q75" s="21"/>
-      <c r="R75" s="21"/>
+      <c r="C75" s="24"/>
+      <c r="D75" s="24"/>
+      <c r="E75" s="24"/>
+      <c r="F75" s="24"/>
+      <c r="G75" s="24"/>
+      <c r="H75" s="24"/>
+      <c r="I75" s="24"/>
+      <c r="J75" s="24"/>
+      <c r="K75" s="24"/>
+      <c r="L75" s="24"/>
+      <c r="M75" s="24"/>
+      <c r="N75" s="24"/>
+      <c r="O75" s="24"/>
+      <c r="P75" s="24"/>
+      <c r="Q75" s="24"/>
+      <c r="R75" s="24"/>
       <c r="S75" s="12"/>
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.2">
@@ -2678,22 +2702,22 @@
         <f t="shared" si="0"/>
         <v>4B0</v>
       </c>
-      <c r="C76" s="21"/>
-      <c r="D76" s="21"/>
-      <c r="E76" s="21"/>
-      <c r="F76" s="21"/>
-      <c r="G76" s="21"/>
-      <c r="H76" s="21"/>
-      <c r="I76" s="21"/>
-      <c r="J76" s="21"/>
-      <c r="K76" s="21"/>
-      <c r="L76" s="21"/>
-      <c r="M76" s="21"/>
-      <c r="N76" s="21"/>
-      <c r="O76" s="21"/>
-      <c r="P76" s="21"/>
-      <c r="Q76" s="21"/>
-      <c r="R76" s="21"/>
+      <c r="C76" s="24"/>
+      <c r="D76" s="24"/>
+      <c r="E76" s="24"/>
+      <c r="F76" s="24"/>
+      <c r="G76" s="24"/>
+      <c r="H76" s="24"/>
+      <c r="I76" s="24"/>
+      <c r="J76" s="24"/>
+      <c r="K76" s="24"/>
+      <c r="L76" s="24"/>
+      <c r="M76" s="24"/>
+      <c r="N76" s="24"/>
+      <c r="O76" s="24"/>
+      <c r="P76" s="24"/>
+      <c r="Q76" s="24"/>
+      <c r="R76" s="24"/>
       <c r="S76" s="12"/>
     </row>
     <row r="77" spans="1:19" x14ac:dyDescent="0.2">
@@ -2704,22 +2728,22 @@
         <f t="shared" si="0"/>
         <v>4C0</v>
       </c>
-      <c r="C77" s="21"/>
-      <c r="D77" s="21"/>
-      <c r="E77" s="21"/>
-      <c r="F77" s="21"/>
-      <c r="G77" s="21"/>
-      <c r="H77" s="21"/>
-      <c r="I77" s="21"/>
-      <c r="J77" s="21"/>
-      <c r="K77" s="21"/>
-      <c r="L77" s="21"/>
-      <c r="M77" s="21"/>
-      <c r="N77" s="21"/>
-      <c r="O77" s="21"/>
-      <c r="P77" s="21"/>
-      <c r="Q77" s="21"/>
-      <c r="R77" s="21"/>
+      <c r="C77" s="24"/>
+      <c r="D77" s="24"/>
+      <c r="E77" s="24"/>
+      <c r="F77" s="24"/>
+      <c r="G77" s="24"/>
+      <c r="H77" s="24"/>
+      <c r="I77" s="24"/>
+      <c r="J77" s="24"/>
+      <c r="K77" s="24"/>
+      <c r="L77" s="24"/>
+      <c r="M77" s="24"/>
+      <c r="N77" s="24"/>
+      <c r="O77" s="24"/>
+      <c r="P77" s="24"/>
+      <c r="Q77" s="24"/>
+      <c r="R77" s="24"/>
       <c r="S77" s="12"/>
     </row>
     <row r="78" spans="1:19" x14ac:dyDescent="0.2">
@@ -2730,22 +2754,22 @@
         <f t="shared" si="0"/>
         <v>4D0</v>
       </c>
-      <c r="C78" s="21"/>
-      <c r="D78" s="21"/>
-      <c r="E78" s="21"/>
-      <c r="F78" s="21"/>
-      <c r="G78" s="21"/>
-      <c r="H78" s="21"/>
-      <c r="I78" s="21"/>
-      <c r="J78" s="21"/>
-      <c r="K78" s="21"/>
-      <c r="L78" s="21"/>
-      <c r="M78" s="21"/>
-      <c r="N78" s="21"/>
-      <c r="O78" s="21"/>
-      <c r="P78" s="21"/>
-      <c r="Q78" s="21"/>
-      <c r="R78" s="21"/>
+      <c r="C78" s="24"/>
+      <c r="D78" s="24"/>
+      <c r="E78" s="24"/>
+      <c r="F78" s="24"/>
+      <c r="G78" s="24"/>
+      <c r="H78" s="24"/>
+      <c r="I78" s="24"/>
+      <c r="J78" s="24"/>
+      <c r="K78" s="24"/>
+      <c r="L78" s="24"/>
+      <c r="M78" s="24"/>
+      <c r="N78" s="24"/>
+      <c r="O78" s="24"/>
+      <c r="P78" s="24"/>
+      <c r="Q78" s="24"/>
+      <c r="R78" s="24"/>
       <c r="S78" s="12"/>
     </row>
     <row r="79" spans="1:19" x14ac:dyDescent="0.2">
@@ -2756,22 +2780,22 @@
         <f t="shared" si="0"/>
         <v>4E0</v>
       </c>
-      <c r="C79" s="21"/>
-      <c r="D79" s="21"/>
-      <c r="E79" s="21"/>
-      <c r="F79" s="21"/>
-      <c r="G79" s="21"/>
-      <c r="H79" s="21"/>
-      <c r="I79" s="21"/>
-      <c r="J79" s="21"/>
-      <c r="K79" s="21"/>
-      <c r="L79" s="21"/>
-      <c r="M79" s="21"/>
-      <c r="N79" s="21"/>
-      <c r="O79" s="21"/>
-      <c r="P79" s="21"/>
-      <c r="Q79" s="21"/>
-      <c r="R79" s="21"/>
+      <c r="C79" s="24"/>
+      <c r="D79" s="24"/>
+      <c r="E79" s="24"/>
+      <c r="F79" s="24"/>
+      <c r="G79" s="24"/>
+      <c r="H79" s="24"/>
+      <c r="I79" s="24"/>
+      <c r="J79" s="24"/>
+      <c r="K79" s="24"/>
+      <c r="L79" s="24"/>
+      <c r="M79" s="24"/>
+      <c r="N79" s="24"/>
+      <c r="O79" s="24"/>
+      <c r="P79" s="24"/>
+      <c r="Q79" s="24"/>
+      <c r="R79" s="24"/>
       <c r="S79" s="12"/>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.2">
@@ -2782,22 +2806,22 @@
         <f t="shared" si="0"/>
         <v>4F0</v>
       </c>
-      <c r="C80" s="21"/>
-      <c r="D80" s="21"/>
-      <c r="E80" s="21"/>
-      <c r="F80" s="21"/>
-      <c r="G80" s="21"/>
-      <c r="H80" s="21"/>
-      <c r="I80" s="21"/>
-      <c r="J80" s="21"/>
-      <c r="K80" s="21"/>
-      <c r="L80" s="21"/>
-      <c r="M80" s="21"/>
-      <c r="N80" s="21"/>
-      <c r="O80" s="21"/>
-      <c r="P80" s="21"/>
-      <c r="Q80" s="21"/>
-      <c r="R80" s="21"/>
+      <c r="C80" s="24"/>
+      <c r="D80" s="24"/>
+      <c r="E80" s="24"/>
+      <c r="F80" s="24"/>
+      <c r="G80" s="24"/>
+      <c r="H80" s="24"/>
+      <c r="I80" s="24"/>
+      <c r="J80" s="24"/>
+      <c r="K80" s="24"/>
+      <c r="L80" s="24"/>
+      <c r="M80" s="24"/>
+      <c r="N80" s="24"/>
+      <c r="O80" s="24"/>
+      <c r="P80" s="24"/>
+      <c r="Q80" s="24"/>
+      <c r="R80" s="24"/>
       <c r="S80" s="12"/>
     </row>
     <row r="81" spans="1:19" x14ac:dyDescent="0.2">
@@ -2808,22 +2832,22 @@
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
-      <c r="C81" s="21"/>
-      <c r="D81" s="21"/>
-      <c r="E81" s="21"/>
-      <c r="F81" s="21"/>
-      <c r="G81" s="21"/>
-      <c r="H81" s="21"/>
-      <c r="I81" s="21"/>
-      <c r="J81" s="21"/>
-      <c r="K81" s="21"/>
-      <c r="L81" s="21"/>
-      <c r="M81" s="21"/>
-      <c r="N81" s="21"/>
-      <c r="O81" s="21"/>
-      <c r="P81" s="21"/>
-      <c r="Q81" s="21"/>
-      <c r="R81" s="21"/>
+      <c r="C81" s="24"/>
+      <c r="D81" s="24"/>
+      <c r="E81" s="24"/>
+      <c r="F81" s="24"/>
+      <c r="G81" s="24"/>
+      <c r="H81" s="24"/>
+      <c r="I81" s="24"/>
+      <c r="J81" s="24"/>
+      <c r="K81" s="24"/>
+      <c r="L81" s="24"/>
+      <c r="M81" s="24"/>
+      <c r="N81" s="24"/>
+      <c r="O81" s="24"/>
+      <c r="P81" s="24"/>
+      <c r="Q81" s="24"/>
+      <c r="R81" s="24"/>
       <c r="S81" s="12"/>
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.2">
@@ -2834,22 +2858,22 @@
         <f t="shared" si="0"/>
         <v>510</v>
       </c>
-      <c r="C82" s="21"/>
-      <c r="D82" s="21"/>
-      <c r="E82" s="21"/>
-      <c r="F82" s="21"/>
-      <c r="G82" s="21"/>
-      <c r="H82" s="21"/>
-      <c r="I82" s="21"/>
-      <c r="J82" s="21"/>
-      <c r="K82" s="21"/>
-      <c r="L82" s="21"/>
-      <c r="M82" s="21"/>
-      <c r="N82" s="21"/>
-      <c r="O82" s="21"/>
-      <c r="P82" s="21"/>
-      <c r="Q82" s="21"/>
-      <c r="R82" s="21"/>
+      <c r="C82" s="24"/>
+      <c r="D82" s="24"/>
+      <c r="E82" s="24"/>
+      <c r="F82" s="24"/>
+      <c r="G82" s="24"/>
+      <c r="H82" s="24"/>
+      <c r="I82" s="24"/>
+      <c r="J82" s="24"/>
+      <c r="K82" s="24"/>
+      <c r="L82" s="24"/>
+      <c r="M82" s="24"/>
+      <c r="N82" s="24"/>
+      <c r="O82" s="24"/>
+      <c r="P82" s="24"/>
+      <c r="Q82" s="24"/>
+      <c r="R82" s="24"/>
       <c r="S82" s="12"/>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.2">
@@ -2860,22 +2884,22 @@
         <f t="shared" si="0"/>
         <v>520</v>
       </c>
-      <c r="C83" s="21"/>
-      <c r="D83" s="21"/>
-      <c r="E83" s="21"/>
-      <c r="F83" s="21"/>
-      <c r="G83" s="21"/>
-      <c r="H83" s="21"/>
-      <c r="I83" s="21"/>
-      <c r="J83" s="21"/>
-      <c r="K83" s="21"/>
-      <c r="L83" s="21"/>
-      <c r="M83" s="21"/>
-      <c r="N83" s="21"/>
-      <c r="O83" s="21"/>
-      <c r="P83" s="21"/>
-      <c r="Q83" s="21"/>
-      <c r="R83" s="21"/>
+      <c r="C83" s="24"/>
+      <c r="D83" s="24"/>
+      <c r="E83" s="24"/>
+      <c r="F83" s="24"/>
+      <c r="G83" s="24"/>
+      <c r="H83" s="24"/>
+      <c r="I83" s="24"/>
+      <c r="J83" s="24"/>
+      <c r="K83" s="24"/>
+      <c r="L83" s="24"/>
+      <c r="M83" s="24"/>
+      <c r="N83" s="24"/>
+      <c r="O83" s="24"/>
+      <c r="P83" s="24"/>
+      <c r="Q83" s="24"/>
+      <c r="R83" s="24"/>
       <c r="S83" s="12"/>
     </row>
     <row r="84" spans="1:19" x14ac:dyDescent="0.2">
@@ -2886,22 +2910,22 @@
         <f t="shared" si="0"/>
         <v>530</v>
       </c>
-      <c r="C84" s="21"/>
-      <c r="D84" s="21"/>
-      <c r="E84" s="21"/>
-      <c r="F84" s="21"/>
-      <c r="G84" s="21"/>
-      <c r="H84" s="21"/>
-      <c r="I84" s="21"/>
-      <c r="J84" s="21"/>
-      <c r="K84" s="21"/>
-      <c r="L84" s="21"/>
-      <c r="M84" s="21"/>
-      <c r="N84" s="21"/>
-      <c r="O84" s="21"/>
-      <c r="P84" s="21"/>
-      <c r="Q84" s="21"/>
-      <c r="R84" s="21"/>
+      <c r="C84" s="24"/>
+      <c r="D84" s="24"/>
+      <c r="E84" s="24"/>
+      <c r="F84" s="24"/>
+      <c r="G84" s="24"/>
+      <c r="H84" s="24"/>
+      <c r="I84" s="24"/>
+      <c r="J84" s="24"/>
+      <c r="K84" s="24"/>
+      <c r="L84" s="24"/>
+      <c r="M84" s="24"/>
+      <c r="N84" s="24"/>
+      <c r="O84" s="24"/>
+      <c r="P84" s="24"/>
+      <c r="Q84" s="24"/>
+      <c r="R84" s="24"/>
       <c r="S84" s="12"/>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.2">
@@ -2912,22 +2936,22 @@
         <f t="shared" si="0"/>
         <v>540</v>
       </c>
-      <c r="C85" s="21"/>
-      <c r="D85" s="21"/>
-      <c r="E85" s="21"/>
-      <c r="F85" s="21"/>
-      <c r="G85" s="21"/>
-      <c r="H85" s="21"/>
-      <c r="I85" s="21"/>
-      <c r="J85" s="21"/>
-      <c r="K85" s="21"/>
-      <c r="L85" s="21"/>
-      <c r="M85" s="21"/>
-      <c r="N85" s="21"/>
-      <c r="O85" s="21"/>
-      <c r="P85" s="21"/>
-      <c r="Q85" s="21"/>
-      <c r="R85" s="21"/>
+      <c r="C85" s="24"/>
+      <c r="D85" s="24"/>
+      <c r="E85" s="24"/>
+      <c r="F85" s="24"/>
+      <c r="G85" s="24"/>
+      <c r="H85" s="24"/>
+      <c r="I85" s="24"/>
+      <c r="J85" s="24"/>
+      <c r="K85" s="24"/>
+      <c r="L85" s="24"/>
+      <c r="M85" s="24"/>
+      <c r="N85" s="24"/>
+      <c r="O85" s="24"/>
+      <c r="P85" s="24"/>
+      <c r="Q85" s="24"/>
+      <c r="R85" s="24"/>
       <c r="S85" s="12"/>
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.2">
@@ -2938,22 +2962,22 @@
         <f t="shared" si="0"/>
         <v>550</v>
       </c>
-      <c r="C86" s="21"/>
-      <c r="D86" s="21"/>
-      <c r="E86" s="21"/>
-      <c r="F86" s="21"/>
-      <c r="G86" s="21"/>
-      <c r="H86" s="21"/>
-      <c r="I86" s="21"/>
-      <c r="J86" s="21"/>
-      <c r="K86" s="21"/>
-      <c r="L86" s="21"/>
-      <c r="M86" s="21"/>
-      <c r="N86" s="21"/>
-      <c r="O86" s="21"/>
-      <c r="P86" s="21"/>
-      <c r="Q86" s="21"/>
-      <c r="R86" s="21"/>
+      <c r="C86" s="24"/>
+      <c r="D86" s="24"/>
+      <c r="E86" s="24"/>
+      <c r="F86" s="24"/>
+      <c r="G86" s="24"/>
+      <c r="H86" s="24"/>
+      <c r="I86" s="24"/>
+      <c r="J86" s="24"/>
+      <c r="K86" s="24"/>
+      <c r="L86" s="24"/>
+      <c r="M86" s="24"/>
+      <c r="N86" s="24"/>
+      <c r="O86" s="24"/>
+      <c r="P86" s="24"/>
+      <c r="Q86" s="24"/>
+      <c r="R86" s="24"/>
       <c r="S86" s="12"/>
     </row>
     <row r="87" spans="1:19" x14ac:dyDescent="0.2">
@@ -2964,22 +2988,22 @@
         <f t="shared" si="0"/>
         <v>560</v>
       </c>
-      <c r="C87" s="22"/>
-      <c r="D87" s="21"/>
-      <c r="E87" s="21"/>
-      <c r="F87" s="21"/>
-      <c r="G87" s="21"/>
-      <c r="H87" s="21"/>
-      <c r="I87" s="21"/>
-      <c r="J87" s="21"/>
+      <c r="C87" s="29"/>
+      <c r="D87" s="24"/>
+      <c r="E87" s="24"/>
+      <c r="F87" s="24"/>
+      <c r="G87" s="24"/>
+      <c r="H87" s="24"/>
+      <c r="I87" s="24"/>
+      <c r="J87" s="24"/>
       <c r="K87" s="10"/>
-      <c r="L87" s="31"/>
-      <c r="M87" s="21"/>
-      <c r="N87" s="21"/>
-      <c r="O87" s="21"/>
-      <c r="P87" s="21"/>
-      <c r="Q87" s="21"/>
-      <c r="R87" s="21"/>
+      <c r="L87" s="30"/>
+      <c r="M87" s="24"/>
+      <c r="N87" s="24"/>
+      <c r="O87" s="24"/>
+      <c r="P87" s="24"/>
+      <c r="Q87" s="24"/>
+      <c r="R87" s="24"/>
       <c r="S87" s="12"/>
     </row>
     <row r="88" spans="1:19" x14ac:dyDescent="0.2">
@@ -2990,24 +3014,24 @@
         <f t="shared" si="0"/>
         <v>570</v>
       </c>
-      <c r="C88" s="32" t="s">
+      <c r="C88" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="D88" s="21"/>
-      <c r="E88" s="21"/>
-      <c r="F88" s="21"/>
-      <c r="G88" s="21"/>
-      <c r="H88" s="21"/>
-      <c r="I88" s="21"/>
-      <c r="J88" s="21"/>
-      <c r="K88" s="21"/>
-      <c r="L88" s="21"/>
-      <c r="M88" s="21"/>
-      <c r="N88" s="21"/>
-      <c r="O88" s="21"/>
-      <c r="P88" s="21"/>
-      <c r="Q88" s="21"/>
-      <c r="R88" s="21"/>
+      <c r="D88" s="24"/>
+      <c r="E88" s="24"/>
+      <c r="F88" s="24"/>
+      <c r="G88" s="24"/>
+      <c r="H88" s="24"/>
+      <c r="I88" s="24"/>
+      <c r="J88" s="24"/>
+      <c r="K88" s="24"/>
+      <c r="L88" s="24"/>
+      <c r="M88" s="24"/>
+      <c r="N88" s="24"/>
+      <c r="O88" s="24"/>
+      <c r="P88" s="24"/>
+      <c r="Q88" s="24"/>
+      <c r="R88" s="24"/>
       <c r="S88" s="12"/>
     </row>
     <row r="89" spans="1:19" x14ac:dyDescent="0.2">
@@ -3018,22 +3042,22 @@
         <f t="shared" si="0"/>
         <v>580</v>
       </c>
-      <c r="C89" s="31"/>
-      <c r="D89" s="21"/>
-      <c r="E89" s="21"/>
-      <c r="F89" s="21"/>
-      <c r="G89" s="21"/>
-      <c r="H89" s="21"/>
-      <c r="I89" s="21"/>
-      <c r="J89" s="21"/>
-      <c r="K89" s="21"/>
-      <c r="L89" s="20"/>
-      <c r="M89" s="21"/>
-      <c r="N89" s="21"/>
-      <c r="O89" s="21"/>
-      <c r="P89" s="21"/>
-      <c r="Q89" s="21"/>
-      <c r="R89" s="21"/>
+      <c r="C89" s="30"/>
+      <c r="D89" s="24"/>
+      <c r="E89" s="24"/>
+      <c r="F89" s="24"/>
+      <c r="G89" s="24"/>
+      <c r="H89" s="24"/>
+      <c r="I89" s="24"/>
+      <c r="J89" s="24"/>
+      <c r="K89" s="24"/>
+      <c r="L89" s="32"/>
+      <c r="M89" s="24"/>
+      <c r="N89" s="24"/>
+      <c r="O89" s="24"/>
+      <c r="P89" s="24"/>
+      <c r="Q89" s="24"/>
+      <c r="R89" s="24"/>
       <c r="S89" s="12"/>
     </row>
     <row r="90" spans="1:19" x14ac:dyDescent="0.2">
@@ -3044,24 +3068,24 @@
         <f t="shared" si="0"/>
         <v>590</v>
       </c>
-      <c r="C90" s="20" t="s">
+      <c r="C90" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="D90" s="21"/>
-      <c r="E90" s="21"/>
-      <c r="F90" s="21"/>
-      <c r="G90" s="21"/>
-      <c r="H90" s="21"/>
-      <c r="I90" s="21"/>
-      <c r="J90" s="21"/>
-      <c r="K90" s="21"/>
-      <c r="L90" s="21"/>
-      <c r="M90" s="21"/>
-      <c r="N90" s="21"/>
-      <c r="O90" s="21"/>
-      <c r="P90" s="21"/>
-      <c r="Q90" s="21"/>
-      <c r="R90" s="21"/>
+      <c r="D90" s="24"/>
+      <c r="E90" s="24"/>
+      <c r="F90" s="24"/>
+      <c r="G90" s="24"/>
+      <c r="H90" s="24"/>
+      <c r="I90" s="24"/>
+      <c r="J90" s="24"/>
+      <c r="K90" s="24"/>
+      <c r="L90" s="24"/>
+      <c r="M90" s="24"/>
+      <c r="N90" s="24"/>
+      <c r="O90" s="24"/>
+      <c r="P90" s="24"/>
+      <c r="Q90" s="24"/>
+      <c r="R90" s="24"/>
       <c r="S90" s="12"/>
     </row>
     <row r="91" spans="1:19" x14ac:dyDescent="0.2">
@@ -3072,22 +3096,22 @@
         <f t="shared" si="0"/>
         <v>5A0</v>
       </c>
-      <c r="C91" s="20"/>
-      <c r="D91" s="21"/>
-      <c r="E91" s="21"/>
-      <c r="F91" s="21"/>
-      <c r="G91" s="21"/>
-      <c r="H91" s="21"/>
-      <c r="I91" s="21"/>
-      <c r="J91" s="21"/>
-      <c r="K91" s="21"/>
+      <c r="C91" s="32"/>
+      <c r="D91" s="24"/>
+      <c r="E91" s="24"/>
+      <c r="F91" s="24"/>
+      <c r="G91" s="24"/>
+      <c r="H91" s="24"/>
+      <c r="I91" s="24"/>
+      <c r="J91" s="24"/>
+      <c r="K91" s="24"/>
       <c r="L91" s="10"/>
       <c r="M91" s="10"/>
       <c r="N91" s="10"/>
-      <c r="O91" s="23" t="s">
+      <c r="O91" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="P91" s="21"/>
+      <c r="P91" s="24"/>
       <c r="Q91" s="10"/>
       <c r="R91" s="10"/>
       <c r="S91" s="12"/>
@@ -3102,28 +3126,28 @@
       </c>
       <c r="E92" s="10"/>
       <c r="F92" s="10"/>
-      <c r="G92" s="28" t="s">
+      <c r="G92" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="H92" s="21"/>
-      <c r="I92" s="26" t="s">
+      <c r="H92" s="24"/>
+      <c r="I92" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="J92" s="21"/>
-      <c r="K92" s="25" t="s">
+      <c r="J92" s="24"/>
+      <c r="K92" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="L92" s="21"/>
-      <c r="M92" s="29" t="s">
+      <c r="L92" s="24"/>
+      <c r="M92" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="N92" s="21"/>
+      <c r="N92" s="24"/>
       <c r="O92" s="10"/>
       <c r="P92" s="10"/>
-      <c r="Q92" s="27" t="s">
+      <c r="Q92" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="R92" s="21"/>
+      <c r="R92" s="24"/>
       <c r="S92" s="12"/>
     </row>
     <row r="93" spans="1:19" x14ac:dyDescent="0.2">
@@ -3134,13 +3158,13 @@
         <f t="shared" si="0"/>
         <v>5C0</v>
       </c>
-      <c r="C93" s="25" t="s">
+      <c r="C93" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="D93" s="21"/>
-      <c r="E93" s="21"/>
-      <c r="F93" s="21"/>
-      <c r="G93" s="21"/>
+      <c r="D93" s="24"/>
+      <c r="E93" s="24"/>
+      <c r="F93" s="24"/>
+      <c r="G93" s="24"/>
       <c r="H93" s="10"/>
       <c r="I93" s="10"/>
       <c r="J93" s="10"/>
@@ -3934,10 +3958,10 @@
       <c r="L123" s="10"/>
       <c r="M123" s="10"/>
       <c r="N123" s="10"/>
-      <c r="O123" s="24"/>
-      <c r="P123" s="21"/>
-      <c r="Q123" s="21"/>
-      <c r="R123" s="21"/>
+      <c r="O123" s="33"/>
+      <c r="P123" s="24"/>
+      <c r="Q123" s="24"/>
+      <c r="R123" s="24"/>
       <c r="S123" s="12"/>
     </row>
     <row r="124" spans="1:19" x14ac:dyDescent="0.2">
@@ -3948,22 +3972,22 @@
         <f t="shared" si="0"/>
         <v>7B0</v>
       </c>
-      <c r="C124" s="24"/>
-      <c r="D124" s="21"/>
-      <c r="E124" s="21"/>
-      <c r="F124" s="21"/>
-      <c r="G124" s="21"/>
-      <c r="H124" s="21"/>
-      <c r="I124" s="21"/>
-      <c r="J124" s="21"/>
-      <c r="K124" s="21"/>
-      <c r="L124" s="21"/>
-      <c r="M124" s="21"/>
-      <c r="N124" s="21"/>
-      <c r="O124" s="21"/>
-      <c r="P124" s="21"/>
-      <c r="Q124" s="21"/>
-      <c r="R124" s="21"/>
+      <c r="C124" s="33"/>
+      <c r="D124" s="24"/>
+      <c r="E124" s="24"/>
+      <c r="F124" s="24"/>
+      <c r="G124" s="24"/>
+      <c r="H124" s="24"/>
+      <c r="I124" s="24"/>
+      <c r="J124" s="24"/>
+      <c r="K124" s="24"/>
+      <c r="L124" s="24"/>
+      <c r="M124" s="24"/>
+      <c r="N124" s="24"/>
+      <c r="O124" s="24"/>
+      <c r="P124" s="24"/>
+      <c r="Q124" s="24"/>
+      <c r="R124" s="24"/>
       <c r="S124" s="12"/>
     </row>
     <row r="125" spans="1:19" x14ac:dyDescent="0.2">
@@ -3974,22 +3998,22 @@
         <f t="shared" si="0"/>
         <v>7C0</v>
       </c>
-      <c r="C125" s="21"/>
-      <c r="D125" s="21"/>
-      <c r="E125" s="21"/>
-      <c r="F125" s="21"/>
-      <c r="G125" s="21"/>
-      <c r="H125" s="21"/>
-      <c r="I125" s="21"/>
-      <c r="J125" s="21"/>
-      <c r="K125" s="21"/>
-      <c r="L125" s="21"/>
-      <c r="M125" s="21"/>
-      <c r="N125" s="21"/>
-      <c r="O125" s="21"/>
-      <c r="P125" s="21"/>
-      <c r="Q125" s="21"/>
-      <c r="R125" s="21"/>
+      <c r="C125" s="24"/>
+      <c r="D125" s="24"/>
+      <c r="E125" s="24"/>
+      <c r="F125" s="24"/>
+      <c r="G125" s="24"/>
+      <c r="H125" s="24"/>
+      <c r="I125" s="24"/>
+      <c r="J125" s="24"/>
+      <c r="K125" s="24"/>
+      <c r="L125" s="24"/>
+      <c r="M125" s="24"/>
+      <c r="N125" s="24"/>
+      <c r="O125" s="24"/>
+      <c r="P125" s="24"/>
+      <c r="Q125" s="24"/>
+      <c r="R125" s="24"/>
       <c r="S125" s="12"/>
     </row>
     <row r="126" spans="1:19" x14ac:dyDescent="0.2">
@@ -4000,22 +4024,22 @@
         <f t="shared" si="0"/>
         <v>7D0</v>
       </c>
-      <c r="C126" s="21"/>
-      <c r="D126" s="21"/>
-      <c r="E126" s="21"/>
-      <c r="F126" s="21"/>
-      <c r="G126" s="21"/>
-      <c r="H126" s="21"/>
-      <c r="I126" s="21"/>
-      <c r="J126" s="21"/>
-      <c r="K126" s="21"/>
-      <c r="L126" s="21"/>
-      <c r="M126" s="21"/>
-      <c r="N126" s="21"/>
-      <c r="O126" s="21"/>
-      <c r="P126" s="21"/>
-      <c r="Q126" s="21"/>
-      <c r="R126" s="21"/>
+      <c r="C126" s="24"/>
+      <c r="D126" s="24"/>
+      <c r="E126" s="24"/>
+      <c r="F126" s="24"/>
+      <c r="G126" s="24"/>
+      <c r="H126" s="24"/>
+      <c r="I126" s="24"/>
+      <c r="J126" s="24"/>
+      <c r="K126" s="24"/>
+      <c r="L126" s="24"/>
+      <c r="M126" s="24"/>
+      <c r="N126" s="24"/>
+      <c r="O126" s="24"/>
+      <c r="P126" s="24"/>
+      <c r="Q126" s="24"/>
+      <c r="R126" s="24"/>
       <c r="S126" s="12"/>
     </row>
     <row r="127" spans="1:19" x14ac:dyDescent="0.2">
@@ -4026,22 +4050,22 @@
         <f t="shared" si="0"/>
         <v>7E0</v>
       </c>
-      <c r="C127" s="21"/>
-      <c r="D127" s="21"/>
-      <c r="E127" s="21"/>
-      <c r="F127" s="21"/>
-      <c r="G127" s="21"/>
-      <c r="H127" s="21"/>
-      <c r="I127" s="21"/>
-      <c r="J127" s="21"/>
-      <c r="K127" s="21"/>
-      <c r="L127" s="21"/>
-      <c r="M127" s="21"/>
-      <c r="N127" s="21"/>
-      <c r="O127" s="21"/>
-      <c r="P127" s="21"/>
-      <c r="Q127" s="21"/>
-      <c r="R127" s="21"/>
+      <c r="C127" s="24"/>
+      <c r="D127" s="24"/>
+      <c r="E127" s="24"/>
+      <c r="F127" s="24"/>
+      <c r="G127" s="24"/>
+      <c r="H127" s="24"/>
+      <c r="I127" s="24"/>
+      <c r="J127" s="24"/>
+      <c r="K127" s="24"/>
+      <c r="L127" s="24"/>
+      <c r="M127" s="24"/>
+      <c r="N127" s="24"/>
+      <c r="O127" s="24"/>
+      <c r="P127" s="24"/>
+      <c r="Q127" s="24"/>
+      <c r="R127" s="24"/>
       <c r="S127" s="12"/>
     </row>
     <row r="128" spans="1:19" x14ac:dyDescent="0.2">
@@ -4052,22 +4076,22 @@
         <f t="shared" si="0"/>
         <v>7F0</v>
       </c>
-      <c r="C128" s="21"/>
-      <c r="D128" s="21"/>
-      <c r="E128" s="21"/>
-      <c r="F128" s="21"/>
-      <c r="G128" s="21"/>
-      <c r="H128" s="21"/>
-      <c r="I128" s="21"/>
-      <c r="J128" s="21"/>
-      <c r="K128" s="21"/>
-      <c r="L128" s="21"/>
-      <c r="M128" s="21"/>
-      <c r="N128" s="21"/>
-      <c r="O128" s="21"/>
-      <c r="P128" s="21"/>
-      <c r="Q128" s="21"/>
-      <c r="R128" s="21"/>
+      <c r="C128" s="24"/>
+      <c r="D128" s="24"/>
+      <c r="E128" s="24"/>
+      <c r="F128" s="24"/>
+      <c r="G128" s="24"/>
+      <c r="H128" s="24"/>
+      <c r="I128" s="24"/>
+      <c r="J128" s="24"/>
+      <c r="K128" s="24"/>
+      <c r="L128" s="24"/>
+      <c r="M128" s="24"/>
+      <c r="N128" s="24"/>
+      <c r="O128" s="24"/>
+      <c r="P128" s="24"/>
+      <c r="Q128" s="24"/>
+      <c r="R128" s="24"/>
       <c r="S128" s="12"/>
     </row>
     <row r="129" spans="1:19" x14ac:dyDescent="0.2">
@@ -14263,19 +14287,20 @@
       <c r="S520" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="C2:M2"/>
-    <mergeCell ref="N2:R2"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="I3:R3"/>
-    <mergeCell ref="K33:N33"/>
-    <mergeCell ref="O33:R33"/>
-    <mergeCell ref="C72:R86"/>
-    <mergeCell ref="C87:J87"/>
-    <mergeCell ref="L87:R87"/>
-    <mergeCell ref="C88:R88"/>
-    <mergeCell ref="C89:K89"/>
-    <mergeCell ref="L89:R89"/>
+  <mergeCells count="36">
+    <mergeCell ref="G50:J50"/>
+    <mergeCell ref="C51:F51"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="K71:R71"/>
+    <mergeCell ref="O34:R34"/>
+    <mergeCell ref="C34:F34"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="K49:N49"/>
+    <mergeCell ref="O49:R49"/>
+    <mergeCell ref="C50:F50"/>
+    <mergeCell ref="O50:R50"/>
+    <mergeCell ref="K35:N35"/>
     <mergeCell ref="C90:R90"/>
     <mergeCell ref="Q92:R92"/>
     <mergeCell ref="O123:R123"/>
@@ -14287,15 +14312,18 @@
     <mergeCell ref="K92:L92"/>
     <mergeCell ref="M92:N92"/>
     <mergeCell ref="C93:G93"/>
-    <mergeCell ref="G50:J50"/>
-    <mergeCell ref="C51:F51"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="K71:R71"/>
-    <mergeCell ref="O34:R34"/>
-    <mergeCell ref="O35:R35"/>
-    <mergeCell ref="C34:F34"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="C72:R86"/>
+    <mergeCell ref="C87:J87"/>
+    <mergeCell ref="L87:R87"/>
+    <mergeCell ref="C88:R88"/>
+    <mergeCell ref="C89:K89"/>
+    <mergeCell ref="L89:R89"/>
+    <mergeCell ref="C2:M2"/>
+    <mergeCell ref="N2:R2"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="I3:R3"/>
+    <mergeCell ref="K33:N33"/>
+    <mergeCell ref="O33:R33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
checkpoint modifying character stats with just darts
</commit_message>
<xml_diff>
--- a/LODEdit/Additional/memory_map.xlsx
+++ b/LODEdit/Additional/memory_map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brett\Documents\memcardrex-plugins-LODEdit\LODEdit\Additional\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DE4F333-88C1-4B57-AD19-001FC3CF86BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9264AA86-98F9-4BAA-BA7A-0680EAD3E29A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15240" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="130">
   <si>
     <t>Address</t>
   </si>
@@ -416,6 +416,12 @@
   <si>
     <t>R4</t>
   </si>
+  <si>
+    <t>L4</t>
+  </si>
+  <si>
+    <t>L5</t>
+  </si>
 </sst>
 </file>
 
@@ -692,7 +698,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -757,87 +763,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -846,22 +776,10 @@
     <xf numFmtId="0" fontId="3" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -870,10 +788,31 @@
     <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -888,13 +827,83 @@
     <xf numFmtId="0" fontId="3" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1118,8 +1127,8 @@
   <dimension ref="A1:T520"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J101" sqref="J101"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S99" sqref="S99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1197,26 +1206,26 @@
         <f t="shared" ref="B2:B520" si="0">DEC2HEX(A2)</f>
         <v>10</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="40" t="s">
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+      <c r="N2" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
+      <c r="O2" s="61"/>
+      <c r="P2" s="61"/>
+      <c r="Q2" s="61"/>
+      <c r="R2" s="61"/>
       <c r="S2" s="6"/>
       <c r="T2" t="s">
         <v>39</v>
@@ -1230,26 +1239,26 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="32" t="s">
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
-      <c r="Q3" s="27"/>
-      <c r="R3" s="27"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
+      <c r="P3" s="61"/>
+      <c r="Q3" s="61"/>
+      <c r="R3" s="61"/>
       <c r="S3" s="6"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
@@ -2022,18 +2031,18 @@
       <c r="H33" s="10"/>
       <c r="I33" s="10"/>
       <c r="J33" s="10"/>
-      <c r="K33" s="32" t="s">
+      <c r="K33" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="L33" s="27"/>
-      <c r="M33" s="27"/>
-      <c r="N33" s="27"/>
-      <c r="O33" s="29" t="s">
+      <c r="L33" s="61"/>
+      <c r="M33" s="61"/>
+      <c r="N33" s="61"/>
+      <c r="O33" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="P33" s="27"/>
-      <c r="Q33" s="27"/>
-      <c r="R33" s="27"/>
+      <c r="P33" s="61"/>
+      <c r="Q33" s="61"/>
+      <c r="R33" s="61"/>
       <c r="S33" s="12"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.2">
@@ -2044,34 +2053,34 @@
         <f t="shared" si="0"/>
         <v>210</v>
       </c>
-      <c r="C34" s="30" t="s">
+      <c r="C34" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="46" t="s">
+      <c r="D34" s="61"/>
+      <c r="E34" s="61"/>
+      <c r="F34" s="61"/>
+      <c r="G34" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="H34" s="60" t="s">
+      <c r="H34" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="I34" s="48" t="s">
+      <c r="I34" s="75" t="s">
         <v>54</v>
       </c>
-      <c r="J34" s="48"/>
-      <c r="K34" s="47" t="s">
+      <c r="J34" s="75"/>
+      <c r="K34" s="76" t="s">
         <v>55</v>
       </c>
-      <c r="L34" s="47"/>
+      <c r="L34" s="76"/>
       <c r="M34" s="10"/>
       <c r="N34" s="10"/>
-      <c r="O34" s="26" t="s">
+      <c r="O34" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="P34" s="27"/>
-      <c r="Q34" s="27"/>
-      <c r="R34" s="27"/>
+      <c r="P34" s="61"/>
+      <c r="Q34" s="61"/>
+      <c r="R34" s="61"/>
       <c r="S34" s="16"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.2">
@@ -2082,24 +2091,24 @@
         <f t="shared" si="0"/>
         <v>220</v>
       </c>
-      <c r="C35" s="28" t="s">
+      <c r="C35" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="D35" s="27"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
+      <c r="D35" s="61"/>
+      <c r="E35" s="61"/>
+      <c r="F35" s="61"/>
       <c r="G35" s="17" t="s">
         <v>16</v>
       </c>
       <c r="H35" s="10"/>
       <c r="I35" s="10"/>
       <c r="J35" s="10"/>
-      <c r="K35" s="33" t="s">
+      <c r="K35" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="L35" s="33"/>
-      <c r="M35" s="33"/>
-      <c r="N35" s="33"/>
+      <c r="L35" s="51"/>
+      <c r="M35" s="51"/>
+      <c r="N35" s="51"/>
       <c r="O35" s="25"/>
       <c r="P35" s="20"/>
       <c r="Q35" s="20"/>
@@ -2462,18 +2471,18 @@
       <c r="H49" s="10"/>
       <c r="I49" s="10"/>
       <c r="J49" s="10"/>
-      <c r="K49" s="32" t="s">
+      <c r="K49" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="L49" s="27"/>
-      <c r="M49" s="27"/>
-      <c r="N49" s="27"/>
-      <c r="O49" s="29" t="s">
+      <c r="L49" s="61"/>
+      <c r="M49" s="61"/>
+      <c r="N49" s="61"/>
+      <c r="O49" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="P49" s="27"/>
-      <c r="Q49" s="27"/>
-      <c r="R49" s="27"/>
+      <c r="P49" s="61"/>
+      <c r="Q49" s="61"/>
+      <c r="R49" s="61"/>
       <c r="S49" s="12"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.2">
@@ -2484,28 +2493,28 @@
         <f t="shared" si="0"/>
         <v>310</v>
       </c>
-      <c r="C50" s="30" t="s">
+      <c r="C50" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="D50" s="27"/>
-      <c r="E50" s="27"/>
-      <c r="F50" s="27"/>
-      <c r="G50" s="26" t="s">
+      <c r="D50" s="61"/>
+      <c r="E50" s="61"/>
+      <c r="F50" s="61"/>
+      <c r="G50" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="H50" s="27"/>
-      <c r="I50" s="27"/>
-      <c r="J50" s="27"/>
+      <c r="H50" s="61"/>
+      <c r="I50" s="61"/>
+      <c r="J50" s="61"/>
       <c r="K50" s="10"/>
       <c r="L50" s="10"/>
       <c r="M50" s="10"/>
       <c r="N50" s="10"/>
-      <c r="O50" s="33" t="s">
+      <c r="O50" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="P50" s="33"/>
-      <c r="Q50" s="33"/>
-      <c r="R50" s="33"/>
+      <c r="P50" s="51"/>
+      <c r="Q50" s="51"/>
+      <c r="R50" s="51"/>
       <c r="S50" s="12"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.2">
@@ -2516,12 +2525,12 @@
         <f t="shared" si="0"/>
         <v>320</v>
       </c>
-      <c r="C51" s="28" t="s">
+      <c r="C51" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="D51" s="27"/>
-      <c r="E51" s="27"/>
-      <c r="F51" s="27"/>
+      <c r="D51" s="61"/>
+      <c r="E51" s="61"/>
+      <c r="F51" s="61"/>
       <c r="G51" s="5" t="s">
         <v>18</v>
       </c>
@@ -2552,10 +2561,10 @@
       <c r="D52" s="10"/>
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
-      <c r="G52" s="29" t="s">
+      <c r="G52" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="H52" s="27"/>
+      <c r="H52" s="61"/>
       <c r="I52" s="10"/>
       <c r="J52" s="10"/>
       <c r="L52" s="10"/>
@@ -3065,14 +3074,14 @@
         <v>25</v>
       </c>
       <c r="J71" s="10"/>
-      <c r="K71" s="28"/>
-      <c r="L71" s="27"/>
-      <c r="M71" s="27"/>
-      <c r="N71" s="27"/>
-      <c r="O71" s="27"/>
-      <c r="P71" s="27"/>
-      <c r="Q71" s="27"/>
-      <c r="R71" s="27"/>
+      <c r="K71" s="66"/>
+      <c r="L71" s="61"/>
+      <c r="M71" s="61"/>
+      <c r="N71" s="61"/>
+      <c r="O71" s="61"/>
+      <c r="P71" s="61"/>
+      <c r="Q71" s="61"/>
+      <c r="R71" s="61"/>
       <c r="S71" s="16" t="s">
         <v>26</v>
       </c>
@@ -3085,24 +3094,24 @@
         <f t="shared" si="0"/>
         <v>470</v>
       </c>
-      <c r="C72" s="37" t="s">
+      <c r="C72" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="D72" s="27"/>
-      <c r="E72" s="27"/>
-      <c r="F72" s="27"/>
-      <c r="G72" s="27"/>
-      <c r="H72" s="27"/>
-      <c r="I72" s="27"/>
-      <c r="J72" s="27"/>
-      <c r="K72" s="27"/>
-      <c r="L72" s="27"/>
-      <c r="M72" s="27"/>
-      <c r="N72" s="27"/>
-      <c r="O72" s="27"/>
-      <c r="P72" s="27"/>
-      <c r="Q72" s="27"/>
-      <c r="R72" s="27"/>
+      <c r="D72" s="61"/>
+      <c r="E72" s="61"/>
+      <c r="F72" s="61"/>
+      <c r="G72" s="61"/>
+      <c r="H72" s="61"/>
+      <c r="I72" s="61"/>
+      <c r="J72" s="61"/>
+      <c r="K72" s="61"/>
+      <c r="L72" s="61"/>
+      <c r="M72" s="61"/>
+      <c r="N72" s="61"/>
+      <c r="O72" s="61"/>
+      <c r="P72" s="61"/>
+      <c r="Q72" s="61"/>
+      <c r="R72" s="61"/>
       <c r="S72" s="12"/>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.2">
@@ -3113,22 +3122,22 @@
         <f t="shared" si="0"/>
         <v>480</v>
       </c>
-      <c r="C73" s="27"/>
-      <c r="D73" s="27"/>
-      <c r="E73" s="27"/>
-      <c r="F73" s="27"/>
-      <c r="G73" s="27"/>
-      <c r="H73" s="27"/>
-      <c r="I73" s="27"/>
-      <c r="J73" s="27"/>
-      <c r="K73" s="27"/>
-      <c r="L73" s="27"/>
-      <c r="M73" s="27"/>
-      <c r="N73" s="27"/>
-      <c r="O73" s="27"/>
-      <c r="P73" s="27"/>
-      <c r="Q73" s="27"/>
-      <c r="R73" s="27"/>
+      <c r="C73" s="61"/>
+      <c r="D73" s="61"/>
+      <c r="E73" s="61"/>
+      <c r="F73" s="61"/>
+      <c r="G73" s="61"/>
+      <c r="H73" s="61"/>
+      <c r="I73" s="61"/>
+      <c r="J73" s="61"/>
+      <c r="K73" s="61"/>
+      <c r="L73" s="61"/>
+      <c r="M73" s="61"/>
+      <c r="N73" s="61"/>
+      <c r="O73" s="61"/>
+      <c r="P73" s="61"/>
+      <c r="Q73" s="61"/>
+      <c r="R73" s="61"/>
       <c r="S73" s="12"/>
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.2">
@@ -3139,22 +3148,22 @@
         <f t="shared" si="0"/>
         <v>490</v>
       </c>
-      <c r="C74" s="27"/>
-      <c r="D74" s="27"/>
-      <c r="E74" s="27"/>
-      <c r="F74" s="27"/>
-      <c r="G74" s="27"/>
-      <c r="H74" s="27"/>
-      <c r="I74" s="27"/>
-      <c r="J74" s="27"/>
-      <c r="K74" s="27"/>
-      <c r="L74" s="27"/>
-      <c r="M74" s="27"/>
-      <c r="N74" s="27"/>
-      <c r="O74" s="27"/>
-      <c r="P74" s="27"/>
-      <c r="Q74" s="27"/>
-      <c r="R74" s="27"/>
+      <c r="C74" s="61"/>
+      <c r="D74" s="61"/>
+      <c r="E74" s="61"/>
+      <c r="F74" s="61"/>
+      <c r="G74" s="61"/>
+      <c r="H74" s="61"/>
+      <c r="I74" s="61"/>
+      <c r="J74" s="61"/>
+      <c r="K74" s="61"/>
+      <c r="L74" s="61"/>
+      <c r="M74" s="61"/>
+      <c r="N74" s="61"/>
+      <c r="O74" s="61"/>
+      <c r="P74" s="61"/>
+      <c r="Q74" s="61"/>
+      <c r="R74" s="61"/>
       <c r="S74" s="12"/>
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.2">
@@ -3165,22 +3174,22 @@
         <f t="shared" si="0"/>
         <v>4A0</v>
       </c>
-      <c r="C75" s="27"/>
-      <c r="D75" s="27"/>
-      <c r="E75" s="27"/>
-      <c r="F75" s="27"/>
-      <c r="G75" s="27"/>
-      <c r="H75" s="27"/>
-      <c r="I75" s="27"/>
-      <c r="J75" s="27"/>
-      <c r="K75" s="27"/>
-      <c r="L75" s="27"/>
-      <c r="M75" s="27"/>
-      <c r="N75" s="27"/>
-      <c r="O75" s="27"/>
-      <c r="P75" s="27"/>
-      <c r="Q75" s="27"/>
-      <c r="R75" s="27"/>
+      <c r="C75" s="61"/>
+      <c r="D75" s="61"/>
+      <c r="E75" s="61"/>
+      <c r="F75" s="61"/>
+      <c r="G75" s="61"/>
+      <c r="H75" s="61"/>
+      <c r="I75" s="61"/>
+      <c r="J75" s="61"/>
+      <c r="K75" s="61"/>
+      <c r="L75" s="61"/>
+      <c r="M75" s="61"/>
+      <c r="N75" s="61"/>
+      <c r="O75" s="61"/>
+      <c r="P75" s="61"/>
+      <c r="Q75" s="61"/>
+      <c r="R75" s="61"/>
       <c r="S75" s="12"/>
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.2">
@@ -3191,22 +3200,22 @@
         <f t="shared" si="0"/>
         <v>4B0</v>
       </c>
-      <c r="C76" s="27"/>
-      <c r="D76" s="27"/>
-      <c r="E76" s="27"/>
-      <c r="F76" s="27"/>
-      <c r="G76" s="27"/>
-      <c r="H76" s="27"/>
-      <c r="I76" s="27"/>
-      <c r="J76" s="27"/>
-      <c r="K76" s="27"/>
-      <c r="L76" s="27"/>
-      <c r="M76" s="27"/>
-      <c r="N76" s="27"/>
-      <c r="O76" s="27"/>
-      <c r="P76" s="27"/>
-      <c r="Q76" s="27"/>
-      <c r="R76" s="27"/>
+      <c r="C76" s="61"/>
+      <c r="D76" s="61"/>
+      <c r="E76" s="61"/>
+      <c r="F76" s="61"/>
+      <c r="G76" s="61"/>
+      <c r="H76" s="61"/>
+      <c r="I76" s="61"/>
+      <c r="J76" s="61"/>
+      <c r="K76" s="61"/>
+      <c r="L76" s="61"/>
+      <c r="M76" s="61"/>
+      <c r="N76" s="61"/>
+      <c r="O76" s="61"/>
+      <c r="P76" s="61"/>
+      <c r="Q76" s="61"/>
+      <c r="R76" s="61"/>
       <c r="S76" s="12"/>
     </row>
     <row r="77" spans="1:19" x14ac:dyDescent="0.2">
@@ -3217,22 +3226,22 @@
         <f t="shared" si="0"/>
         <v>4C0</v>
       </c>
-      <c r="C77" s="27"/>
-      <c r="D77" s="27"/>
-      <c r="E77" s="27"/>
-      <c r="F77" s="27"/>
-      <c r="G77" s="27"/>
-      <c r="H77" s="27"/>
-      <c r="I77" s="27"/>
-      <c r="J77" s="27"/>
-      <c r="K77" s="27"/>
-      <c r="L77" s="27"/>
-      <c r="M77" s="27"/>
-      <c r="N77" s="27"/>
-      <c r="O77" s="27"/>
-      <c r="P77" s="27"/>
-      <c r="Q77" s="27"/>
-      <c r="R77" s="27"/>
+      <c r="C77" s="61"/>
+      <c r="D77" s="61"/>
+      <c r="E77" s="61"/>
+      <c r="F77" s="61"/>
+      <c r="G77" s="61"/>
+      <c r="H77" s="61"/>
+      <c r="I77" s="61"/>
+      <c r="J77" s="61"/>
+      <c r="K77" s="61"/>
+      <c r="L77" s="61"/>
+      <c r="M77" s="61"/>
+      <c r="N77" s="61"/>
+      <c r="O77" s="61"/>
+      <c r="P77" s="61"/>
+      <c r="Q77" s="61"/>
+      <c r="R77" s="61"/>
       <c r="S77" s="12"/>
     </row>
     <row r="78" spans="1:19" x14ac:dyDescent="0.2">
@@ -3243,22 +3252,22 @@
         <f t="shared" si="0"/>
         <v>4D0</v>
       </c>
-      <c r="C78" s="27"/>
-      <c r="D78" s="27"/>
-      <c r="E78" s="27"/>
-      <c r="F78" s="27"/>
-      <c r="G78" s="27"/>
-      <c r="H78" s="27"/>
-      <c r="I78" s="27"/>
-      <c r="J78" s="27"/>
-      <c r="K78" s="27"/>
-      <c r="L78" s="27"/>
-      <c r="M78" s="27"/>
-      <c r="N78" s="27"/>
-      <c r="O78" s="27"/>
-      <c r="P78" s="27"/>
-      <c r="Q78" s="27"/>
-      <c r="R78" s="27"/>
+      <c r="C78" s="61"/>
+      <c r="D78" s="61"/>
+      <c r="E78" s="61"/>
+      <c r="F78" s="61"/>
+      <c r="G78" s="61"/>
+      <c r="H78" s="61"/>
+      <c r="I78" s="61"/>
+      <c r="J78" s="61"/>
+      <c r="K78" s="61"/>
+      <c r="L78" s="61"/>
+      <c r="M78" s="61"/>
+      <c r="N78" s="61"/>
+      <c r="O78" s="61"/>
+      <c r="P78" s="61"/>
+      <c r="Q78" s="61"/>
+      <c r="R78" s="61"/>
       <c r="S78" s="12"/>
     </row>
     <row r="79" spans="1:19" x14ac:dyDescent="0.2">
@@ -3269,22 +3278,22 @@
         <f t="shared" si="0"/>
         <v>4E0</v>
       </c>
-      <c r="C79" s="27"/>
-      <c r="D79" s="27"/>
-      <c r="E79" s="27"/>
-      <c r="F79" s="27"/>
-      <c r="G79" s="27"/>
-      <c r="H79" s="27"/>
-      <c r="I79" s="27"/>
-      <c r="J79" s="27"/>
-      <c r="K79" s="27"/>
-      <c r="L79" s="27"/>
-      <c r="M79" s="27"/>
-      <c r="N79" s="27"/>
-      <c r="O79" s="27"/>
-      <c r="P79" s="27"/>
-      <c r="Q79" s="27"/>
-      <c r="R79" s="27"/>
+      <c r="C79" s="61"/>
+      <c r="D79" s="61"/>
+      <c r="E79" s="61"/>
+      <c r="F79" s="61"/>
+      <c r="G79" s="61"/>
+      <c r="H79" s="61"/>
+      <c r="I79" s="61"/>
+      <c r="J79" s="61"/>
+      <c r="K79" s="61"/>
+      <c r="L79" s="61"/>
+      <c r="M79" s="61"/>
+      <c r="N79" s="61"/>
+      <c r="O79" s="61"/>
+      <c r="P79" s="61"/>
+      <c r="Q79" s="61"/>
+      <c r="R79" s="61"/>
       <c r="S79" s="12"/>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.2">
@@ -3295,22 +3304,22 @@
         <f t="shared" si="0"/>
         <v>4F0</v>
       </c>
-      <c r="C80" s="27"/>
-      <c r="D80" s="27"/>
-      <c r="E80" s="27"/>
-      <c r="F80" s="27"/>
-      <c r="G80" s="27"/>
-      <c r="H80" s="27"/>
-      <c r="I80" s="27"/>
-      <c r="J80" s="27"/>
-      <c r="K80" s="27"/>
-      <c r="L80" s="27"/>
-      <c r="M80" s="27"/>
-      <c r="N80" s="27"/>
-      <c r="O80" s="27"/>
-      <c r="P80" s="27"/>
-      <c r="Q80" s="27"/>
-      <c r="R80" s="27"/>
+      <c r="C80" s="61"/>
+      <c r="D80" s="61"/>
+      <c r="E80" s="61"/>
+      <c r="F80" s="61"/>
+      <c r="G80" s="61"/>
+      <c r="H80" s="61"/>
+      <c r="I80" s="61"/>
+      <c r="J80" s="61"/>
+      <c r="K80" s="61"/>
+      <c r="L80" s="61"/>
+      <c r="M80" s="61"/>
+      <c r="N80" s="61"/>
+      <c r="O80" s="61"/>
+      <c r="P80" s="61"/>
+      <c r="Q80" s="61"/>
+      <c r="R80" s="61"/>
       <c r="S80" s="12"/>
     </row>
     <row r="81" spans="1:19" x14ac:dyDescent="0.2">
@@ -3321,22 +3330,22 @@
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
-      <c r="C81" s="27"/>
-      <c r="D81" s="27"/>
-      <c r="E81" s="27"/>
-      <c r="F81" s="27"/>
-      <c r="G81" s="27"/>
-      <c r="H81" s="27"/>
-      <c r="I81" s="27"/>
-      <c r="J81" s="27"/>
-      <c r="K81" s="27"/>
-      <c r="L81" s="27"/>
-      <c r="M81" s="27"/>
-      <c r="N81" s="27"/>
-      <c r="O81" s="27"/>
-      <c r="P81" s="27"/>
-      <c r="Q81" s="27"/>
-      <c r="R81" s="27"/>
+      <c r="C81" s="61"/>
+      <c r="D81" s="61"/>
+      <c r="E81" s="61"/>
+      <c r="F81" s="61"/>
+      <c r="G81" s="61"/>
+      <c r="H81" s="61"/>
+      <c r="I81" s="61"/>
+      <c r="J81" s="61"/>
+      <c r="K81" s="61"/>
+      <c r="L81" s="61"/>
+      <c r="M81" s="61"/>
+      <c r="N81" s="61"/>
+      <c r="O81" s="61"/>
+      <c r="P81" s="61"/>
+      <c r="Q81" s="61"/>
+      <c r="R81" s="61"/>
       <c r="S81" s="12"/>
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.2">
@@ -3347,22 +3356,22 @@
         <f t="shared" si="0"/>
         <v>510</v>
       </c>
-      <c r="C82" s="27"/>
-      <c r="D82" s="27"/>
-      <c r="E82" s="27"/>
-      <c r="F82" s="27"/>
-      <c r="G82" s="27"/>
-      <c r="H82" s="27"/>
-      <c r="I82" s="27"/>
-      <c r="J82" s="27"/>
-      <c r="K82" s="27"/>
-      <c r="L82" s="27"/>
-      <c r="M82" s="27"/>
-      <c r="N82" s="27"/>
-      <c r="O82" s="27"/>
-      <c r="P82" s="27"/>
-      <c r="Q82" s="27"/>
-      <c r="R82" s="27"/>
+      <c r="C82" s="61"/>
+      <c r="D82" s="61"/>
+      <c r="E82" s="61"/>
+      <c r="F82" s="61"/>
+      <c r="G82" s="61"/>
+      <c r="H82" s="61"/>
+      <c r="I82" s="61"/>
+      <c r="J82" s="61"/>
+      <c r="K82" s="61"/>
+      <c r="L82" s="61"/>
+      <c r="M82" s="61"/>
+      <c r="N82" s="61"/>
+      <c r="O82" s="61"/>
+      <c r="P82" s="61"/>
+      <c r="Q82" s="61"/>
+      <c r="R82" s="61"/>
       <c r="S82" s="12"/>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.2">
@@ -3373,22 +3382,22 @@
         <f t="shared" si="0"/>
         <v>520</v>
       </c>
-      <c r="C83" s="27"/>
-      <c r="D83" s="27"/>
-      <c r="E83" s="27"/>
-      <c r="F83" s="27"/>
-      <c r="G83" s="27"/>
-      <c r="H83" s="27"/>
-      <c r="I83" s="27"/>
-      <c r="J83" s="27"/>
-      <c r="K83" s="27"/>
-      <c r="L83" s="27"/>
-      <c r="M83" s="27"/>
-      <c r="N83" s="27"/>
-      <c r="O83" s="27"/>
-      <c r="P83" s="27"/>
-      <c r="Q83" s="27"/>
-      <c r="R83" s="27"/>
+      <c r="C83" s="61"/>
+      <c r="D83" s="61"/>
+      <c r="E83" s="61"/>
+      <c r="F83" s="61"/>
+      <c r="G83" s="61"/>
+      <c r="H83" s="61"/>
+      <c r="I83" s="61"/>
+      <c r="J83" s="61"/>
+      <c r="K83" s="61"/>
+      <c r="L83" s="61"/>
+      <c r="M83" s="61"/>
+      <c r="N83" s="61"/>
+      <c r="O83" s="61"/>
+      <c r="P83" s="61"/>
+      <c r="Q83" s="61"/>
+      <c r="R83" s="61"/>
       <c r="S83" s="12"/>
     </row>
     <row r="84" spans="1:19" x14ac:dyDescent="0.2">
@@ -3399,22 +3408,22 @@
         <f t="shared" si="0"/>
         <v>530</v>
       </c>
-      <c r="C84" s="27"/>
-      <c r="D84" s="27"/>
-      <c r="E84" s="27"/>
-      <c r="F84" s="27"/>
-      <c r="G84" s="27"/>
-      <c r="H84" s="27"/>
-      <c r="I84" s="27"/>
-      <c r="J84" s="27"/>
-      <c r="K84" s="27"/>
-      <c r="L84" s="27"/>
-      <c r="M84" s="27"/>
-      <c r="N84" s="27"/>
-      <c r="O84" s="27"/>
-      <c r="P84" s="27"/>
-      <c r="Q84" s="27"/>
-      <c r="R84" s="27"/>
+      <c r="C84" s="61"/>
+      <c r="D84" s="61"/>
+      <c r="E84" s="61"/>
+      <c r="F84" s="61"/>
+      <c r="G84" s="61"/>
+      <c r="H84" s="61"/>
+      <c r="I84" s="61"/>
+      <c r="J84" s="61"/>
+      <c r="K84" s="61"/>
+      <c r="L84" s="61"/>
+      <c r="M84" s="61"/>
+      <c r="N84" s="61"/>
+      <c r="O84" s="61"/>
+      <c r="P84" s="61"/>
+      <c r="Q84" s="61"/>
+      <c r="R84" s="61"/>
       <c r="S84" s="12"/>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.2">
@@ -3425,22 +3434,22 @@
         <f t="shared" si="0"/>
         <v>540</v>
       </c>
-      <c r="C85" s="27"/>
-      <c r="D85" s="27"/>
-      <c r="E85" s="27"/>
-      <c r="F85" s="27"/>
-      <c r="G85" s="27"/>
-      <c r="H85" s="27"/>
-      <c r="I85" s="27"/>
-      <c r="J85" s="27"/>
-      <c r="K85" s="27"/>
-      <c r="L85" s="27"/>
-      <c r="M85" s="27"/>
-      <c r="N85" s="27"/>
-      <c r="O85" s="27"/>
-      <c r="P85" s="27"/>
-      <c r="Q85" s="27"/>
-      <c r="R85" s="27"/>
+      <c r="C85" s="61"/>
+      <c r="D85" s="61"/>
+      <c r="E85" s="61"/>
+      <c r="F85" s="61"/>
+      <c r="G85" s="61"/>
+      <c r="H85" s="61"/>
+      <c r="I85" s="61"/>
+      <c r="J85" s="61"/>
+      <c r="K85" s="61"/>
+      <c r="L85" s="61"/>
+      <c r="M85" s="61"/>
+      <c r="N85" s="61"/>
+      <c r="O85" s="61"/>
+      <c r="P85" s="61"/>
+      <c r="Q85" s="61"/>
+      <c r="R85" s="61"/>
       <c r="S85" s="12"/>
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.2">
@@ -3451,22 +3460,22 @@
         <f t="shared" si="0"/>
         <v>550</v>
       </c>
-      <c r="C86" s="27"/>
-      <c r="D86" s="27"/>
-      <c r="E86" s="27"/>
-      <c r="F86" s="27"/>
-      <c r="G86" s="27"/>
-      <c r="H86" s="27"/>
-      <c r="I86" s="27"/>
-      <c r="J86" s="27"/>
-      <c r="K86" s="27"/>
-      <c r="L86" s="27"/>
-      <c r="M86" s="27"/>
-      <c r="N86" s="27"/>
-      <c r="O86" s="27"/>
-      <c r="P86" s="27"/>
-      <c r="Q86" s="27"/>
-      <c r="R86" s="27"/>
+      <c r="C86" s="61"/>
+      <c r="D86" s="61"/>
+      <c r="E86" s="61"/>
+      <c r="F86" s="61"/>
+      <c r="G86" s="61"/>
+      <c r="H86" s="61"/>
+      <c r="I86" s="61"/>
+      <c r="J86" s="61"/>
+      <c r="K86" s="61"/>
+      <c r="L86" s="61"/>
+      <c r="M86" s="61"/>
+      <c r="N86" s="61"/>
+      <c r="O86" s="61"/>
+      <c r="P86" s="61"/>
+      <c r="Q86" s="61"/>
+      <c r="R86" s="61"/>
       <c r="S86" s="12"/>
     </row>
     <row r="87" spans="1:19" x14ac:dyDescent="0.2">
@@ -3477,22 +3486,22 @@
         <f t="shared" si="0"/>
         <v>560</v>
       </c>
-      <c r="C87" s="28"/>
-      <c r="D87" s="27"/>
-      <c r="E87" s="27"/>
-      <c r="F87" s="27"/>
-      <c r="G87" s="27"/>
-      <c r="H87" s="27"/>
-      <c r="I87" s="27"/>
-      <c r="J87" s="27"/>
+      <c r="C87" s="66"/>
+      <c r="D87" s="61"/>
+      <c r="E87" s="61"/>
+      <c r="F87" s="61"/>
+      <c r="G87" s="61"/>
+      <c r="H87" s="61"/>
+      <c r="I87" s="61"/>
+      <c r="J87" s="61"/>
       <c r="K87" s="10"/>
-      <c r="L87" s="38"/>
-      <c r="M87" s="27"/>
-      <c r="N87" s="27"/>
-      <c r="O87" s="27"/>
-      <c r="P87" s="27"/>
-      <c r="Q87" s="27"/>
-      <c r="R87" s="27"/>
+      <c r="L87" s="67"/>
+      <c r="M87" s="61"/>
+      <c r="N87" s="61"/>
+      <c r="O87" s="61"/>
+      <c r="P87" s="61"/>
+      <c r="Q87" s="61"/>
+      <c r="R87" s="61"/>
       <c r="S87" s="12"/>
     </row>
     <row r="88" spans="1:19" x14ac:dyDescent="0.2">
@@ -3503,24 +3512,24 @@
         <f t="shared" si="0"/>
         <v>570</v>
       </c>
-      <c r="C88" s="39" t="s">
+      <c r="C88" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="D88" s="27"/>
-      <c r="E88" s="27"/>
-      <c r="F88" s="27"/>
-      <c r="G88" s="27"/>
-      <c r="H88" s="27"/>
-      <c r="I88" s="27"/>
-      <c r="J88" s="27"/>
-      <c r="K88" s="27"/>
-      <c r="L88" s="27"/>
-      <c r="M88" s="27"/>
-      <c r="N88" s="27"/>
-      <c r="O88" s="27"/>
-      <c r="P88" s="27"/>
-      <c r="Q88" s="27"/>
-      <c r="R88" s="27"/>
+      <c r="D88" s="61"/>
+      <c r="E88" s="61"/>
+      <c r="F88" s="61"/>
+      <c r="G88" s="61"/>
+      <c r="H88" s="61"/>
+      <c r="I88" s="61"/>
+      <c r="J88" s="61"/>
+      <c r="K88" s="61"/>
+      <c r="L88" s="61"/>
+      <c r="M88" s="61"/>
+      <c r="N88" s="61"/>
+      <c r="O88" s="61"/>
+      <c r="P88" s="61"/>
+      <c r="Q88" s="61"/>
+      <c r="R88" s="61"/>
       <c r="S88" s="12"/>
     </row>
     <row r="89" spans="1:19" x14ac:dyDescent="0.2">
@@ -3531,22 +3540,22 @@
         <f t="shared" si="0"/>
         <v>580</v>
       </c>
-      <c r="C89" s="38"/>
-      <c r="D89" s="27"/>
-      <c r="E89" s="27"/>
-      <c r="F89" s="27"/>
-      <c r="G89" s="27"/>
-      <c r="H89" s="27"/>
-      <c r="I89" s="27"/>
-      <c r="J89" s="27"/>
-      <c r="K89" s="27"/>
-      <c r="L89" s="26"/>
-      <c r="M89" s="27"/>
-      <c r="N89" s="27"/>
-      <c r="O89" s="27"/>
-      <c r="P89" s="27"/>
-      <c r="Q89" s="27"/>
-      <c r="R89" s="27"/>
+      <c r="C89" s="67"/>
+      <c r="D89" s="61"/>
+      <c r="E89" s="61"/>
+      <c r="F89" s="61"/>
+      <c r="G89" s="61"/>
+      <c r="H89" s="61"/>
+      <c r="I89" s="61"/>
+      <c r="J89" s="61"/>
+      <c r="K89" s="61"/>
+      <c r="L89" s="69"/>
+      <c r="M89" s="61"/>
+      <c r="N89" s="61"/>
+      <c r="O89" s="61"/>
+      <c r="P89" s="61"/>
+      <c r="Q89" s="61"/>
+      <c r="R89" s="61"/>
       <c r="S89" s="12"/>
     </row>
     <row r="90" spans="1:19" x14ac:dyDescent="0.2">
@@ -3557,24 +3566,24 @@
         <f t="shared" si="0"/>
         <v>590</v>
       </c>
-      <c r="C90" s="26" t="s">
+      <c r="C90" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="D90" s="27"/>
-      <c r="E90" s="27"/>
-      <c r="F90" s="27"/>
-      <c r="G90" s="27"/>
-      <c r="H90" s="27"/>
-      <c r="I90" s="27"/>
-      <c r="J90" s="27"/>
-      <c r="K90" s="27"/>
-      <c r="L90" s="27"/>
-      <c r="M90" s="27"/>
-      <c r="N90" s="27"/>
-      <c r="O90" s="27"/>
-      <c r="P90" s="27"/>
-      <c r="Q90" s="27"/>
-      <c r="R90" s="27"/>
+      <c r="D90" s="61"/>
+      <c r="E90" s="61"/>
+      <c r="F90" s="61"/>
+      <c r="G90" s="61"/>
+      <c r="H90" s="61"/>
+      <c r="I90" s="61"/>
+      <c r="J90" s="61"/>
+      <c r="K90" s="61"/>
+      <c r="L90" s="61"/>
+      <c r="M90" s="61"/>
+      <c r="N90" s="61"/>
+      <c r="O90" s="61"/>
+      <c r="P90" s="61"/>
+      <c r="Q90" s="61"/>
+      <c r="R90" s="61"/>
       <c r="S90" s="12"/>
     </row>
     <row r="91" spans="1:19" x14ac:dyDescent="0.2">
@@ -3585,24 +3594,24 @@
         <f t="shared" si="0"/>
         <v>5A0</v>
       </c>
-      <c r="C91" s="26"/>
-      <c r="D91" s="27"/>
-      <c r="E91" s="27"/>
-      <c r="F91" s="27"/>
-      <c r="G91" s="27"/>
-      <c r="H91" s="27"/>
-      <c r="I91" s="27"/>
-      <c r="J91" s="27"/>
-      <c r="K91" s="27"/>
+      <c r="C91" s="69"/>
+      <c r="D91" s="61"/>
+      <c r="E91" s="61"/>
+      <c r="F91" s="61"/>
+      <c r="G91" s="61"/>
+      <c r="H91" s="61"/>
+      <c r="I91" s="61"/>
+      <c r="J91" s="61"/>
+      <c r="K91" s="61"/>
       <c r="L91" s="10"/>
       <c r="M91" s="10"/>
       <c r="N91" s="10"/>
-      <c r="O91" s="45" t="s">
+      <c r="O91" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="P91" s="45"/>
-      <c r="Q91" s="45"/>
-      <c r="R91" s="45"/>
+      <c r="P91" s="55"/>
+      <c r="Q91" s="55"/>
+      <c r="R91" s="55"/>
       <c r="S91" s="12"/>
     </row>
     <row r="92" spans="1:19" x14ac:dyDescent="0.2">
@@ -3615,28 +3624,28 @@
       </c>
       <c r="E92" s="10"/>
       <c r="F92" s="10"/>
-      <c r="G92" s="35" t="s">
+      <c r="G92" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="H92" s="27"/>
-      <c r="I92" s="31" t="s">
+      <c r="H92" s="61"/>
+      <c r="I92" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="J92" s="27"/>
-      <c r="K92" s="30" t="s">
+      <c r="J92" s="61"/>
+      <c r="K92" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="L92" s="27"/>
-      <c r="M92" s="36" t="s">
+      <c r="L92" s="61"/>
+      <c r="M92" s="73" t="s">
         <v>33</v>
       </c>
-      <c r="N92" s="27"/>
+      <c r="N92" s="61"/>
       <c r="O92" s="10"/>
       <c r="P92" s="10"/>
-      <c r="Q92" s="58" t="s">
+      <c r="Q92" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="R92" s="59" t="s">
+      <c r="R92" s="32" t="s">
         <v>71</v>
       </c>
       <c r="S92" s="12"/>
@@ -3649,13 +3658,13 @@
         <f t="shared" si="0"/>
         <v>5C0</v>
       </c>
-      <c r="C93" s="30" t="s">
+      <c r="C93" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="D93" s="27"/>
-      <c r="E93" s="27"/>
-      <c r="F93" s="27"/>
-      <c r="G93" s="27"/>
+      <c r="D93" s="61"/>
+      <c r="E93" s="61"/>
+      <c r="F93" s="61"/>
+      <c r="G93" s="61"/>
       <c r="H93" s="10"/>
       <c r="I93" s="10"/>
       <c r="J93" s="10"/>
@@ -3701,12 +3710,12 @@
       <c r="H94" s="10"/>
       <c r="I94" s="10"/>
       <c r="J94" s="10"/>
-      <c r="K94" s="43" t="s">
+      <c r="K94" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="L94" s="43"/>
-      <c r="M94" s="43"/>
-      <c r="N94" s="43"/>
+      <c r="L94" s="53"/>
+      <c r="M94" s="53"/>
+      <c r="N94" s="53"/>
       <c r="O94" s="10"/>
       <c r="P94" s="10"/>
       <c r="Q94" s="10"/>
@@ -3721,28 +3730,28 @@
         <f t="shared" si="0"/>
         <v>5E0</v>
       </c>
-      <c r="C95" s="43" t="s">
+      <c r="C95" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="D95" s="43"/>
-      <c r="E95" s="55" t="s">
+      <c r="D95" s="53"/>
+      <c r="E95" s="52" t="s">
         <v>58</v>
       </c>
-      <c r="F95" s="55"/>
-      <c r="G95" s="56" t="s">
+      <c r="F95" s="52"/>
+      <c r="G95" s="59" t="s">
         <v>59</v>
       </c>
-      <c r="H95" s="56"/>
-      <c r="I95" s="55" t="s">
+      <c r="H95" s="59"/>
+      <c r="I95" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="J95" s="55"/>
+      <c r="J95" s="52"/>
       <c r="K95" s="22"/>
       <c r="L95" s="22"/>
-      <c r="M95" s="57" t="s">
+      <c r="M95" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="N95" s="54" t="s">
+      <c r="N95" s="29" t="s">
         <v>60</v>
       </c>
       <c r="O95" s="10"/>
@@ -3778,8 +3787,12 @@
       <c r="O96" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="P96" s="10"/>
-      <c r="Q96" s="10"/>
+      <c r="P96" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q96" s="26" t="s">
+        <v>129</v>
+      </c>
       <c r="R96" s="10"/>
       <c r="S96" s="12"/>
     </row>
@@ -3795,24 +3808,24 @@
       <c r="D97" s="10"/>
       <c r="E97" s="10"/>
       <c r="F97" s="10"/>
-      <c r="G97" s="42" t="s">
+      <c r="G97" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="H97" s="42"/>
-      <c r="I97" s="42"/>
-      <c r="J97" s="42"/>
+      <c r="H97" s="74"/>
+      <c r="I97" s="74"/>
+      <c r="J97" s="74"/>
       <c r="K97" s="10"/>
       <c r="L97" s="10"/>
       <c r="M97" s="10"/>
       <c r="N97" s="10"/>
-      <c r="O97" s="51" t="s">
+      <c r="O97" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="P97" s="50"/>
-      <c r="Q97" s="61" t="s">
+      <c r="P97" s="42"/>
+      <c r="Q97" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="R97" s="61"/>
+      <c r="R97" s="44"/>
       <c r="S97" s="12"/>
     </row>
     <row r="98" spans="1:19" x14ac:dyDescent="0.2">
@@ -3823,20 +3836,20 @@
         <f t="shared" si="0"/>
         <v>610</v>
       </c>
-      <c r="C98" s="61" t="s">
+      <c r="C98" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="D98" s="61"/>
-      <c r="E98" s="62" t="s">
+      <c r="D98" s="44"/>
+      <c r="E98" s="54" t="s">
         <v>80</v>
       </c>
-      <c r="F98" s="62"/>
+      <c r="F98" s="54"/>
       <c r="G98" s="10"/>
       <c r="H98" s="10"/>
-      <c r="I98" s="63" t="s">
+      <c r="I98" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="J98" s="49" t="s">
+      <c r="J98" s="28" t="s">
         <v>82</v>
       </c>
       <c r="K98" s="10"/>
@@ -3883,32 +3896,32 @@
         <f t="shared" si="0"/>
         <v>630</v>
       </c>
-      <c r="C100" s="33" t="s">
+      <c r="C100" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="D100" s="33"/>
-      <c r="E100" s="33"/>
-      <c r="F100" s="33"/>
+      <c r="D100" s="51"/>
+      <c r="E100" s="51"/>
+      <c r="F100" s="51"/>
       <c r="G100" s="10"/>
       <c r="H100" s="10"/>
       <c r="I100" s="10"/>
       <c r="J100" s="10"/>
-      <c r="K100" s="52" t="s">
+      <c r="K100" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="L100" s="33"/>
-      <c r="M100" s="64" t="s">
+      <c r="L100" s="51"/>
+      <c r="M100" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="N100" s="64"/>
-      <c r="O100" s="33" t="s">
+      <c r="N100" s="50"/>
+      <c r="O100" s="51" t="s">
         <v>84</v>
       </c>
-      <c r="P100" s="33"/>
-      <c r="Q100" s="64" t="s">
+      <c r="P100" s="51"/>
+      <c r="Q100" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="R100" s="64"/>
+      <c r="R100" s="50"/>
       <c r="S100" s="12"/>
     </row>
     <row r="101" spans="1:19" x14ac:dyDescent="0.2">
@@ -3924,7 +3937,7 @@
       <c r="E101" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="F101" s="65" t="s">
+      <c r="F101" s="35" t="s">
         <v>87</v>
       </c>
       <c r="G101" s="10"/>
@@ -3969,12 +3982,12 @@
       <c r="L102" s="10"/>
       <c r="M102" s="10"/>
       <c r="N102" s="10"/>
-      <c r="O102" s="33" t="s">
+      <c r="O102" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="P102" s="33"/>
-      <c r="Q102" s="33"/>
-      <c r="R102" s="33"/>
+      <c r="P102" s="51"/>
+      <c r="Q102" s="51"/>
+      <c r="R102" s="51"/>
       <c r="S102" s="12"/>
     </row>
     <row r="103" spans="1:19" x14ac:dyDescent="0.2">
@@ -3989,28 +4002,28 @@
       <c r="D103" s="10"/>
       <c r="E103" s="10"/>
       <c r="F103" s="10"/>
-      <c r="G103" s="33" t="s">
+      <c r="G103" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="H103" s="33"/>
-      <c r="I103" s="64" t="s">
+      <c r="H103" s="51"/>
+      <c r="I103" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="J103" s="64"/>
-      <c r="K103" s="33" t="s">
+      <c r="J103" s="50"/>
+      <c r="K103" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="L103" s="33"/>
-      <c r="M103" s="64" t="s">
+      <c r="L103" s="51"/>
+      <c r="M103" s="50" t="s">
         <v>90</v>
       </c>
-      <c r="N103" s="64"/>
+      <c r="N103" s="50"/>
       <c r="O103" s="10"/>
       <c r="P103" s="10"/>
       <c r="Q103" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="R103" s="65" t="s">
+      <c r="R103" s="35" t="s">
         <v>92</v>
       </c>
       <c r="S103" s="12"/>
@@ -4069,12 +4082,12 @@
       <c r="H105" s="10"/>
       <c r="I105" s="10"/>
       <c r="J105" s="10"/>
-      <c r="K105" s="43" t="s">
+      <c r="K105" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="L105" s="43"/>
-      <c r="M105" s="43"/>
-      <c r="N105" s="43"/>
+      <c r="L105" s="53"/>
+      <c r="M105" s="53"/>
+      <c r="N105" s="53"/>
       <c r="O105" s="10"/>
       <c r="P105" s="10"/>
       <c r="Q105" s="10"/>
@@ -4089,28 +4102,28 @@
         <f t="shared" si="0"/>
         <v>690</v>
       </c>
-      <c r="C106" s="43" t="s">
+      <c r="C106" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="D106" s="43"/>
-      <c r="E106" s="55" t="s">
+      <c r="D106" s="53"/>
+      <c r="E106" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="F106" s="55"/>
-      <c r="G106" s="43" t="s">
+      <c r="F106" s="52"/>
+      <c r="G106" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="H106" s="43"/>
-      <c r="I106" s="55" t="s">
+      <c r="H106" s="53"/>
+      <c r="I106" s="52" t="s">
         <v>95</v>
       </c>
-      <c r="J106" s="55"/>
+      <c r="J106" s="52"/>
       <c r="K106" s="10"/>
       <c r="L106" s="10"/>
-      <c r="M106" s="66" t="s">
+      <c r="M106" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="N106" s="54" t="s">
+      <c r="N106" s="29" t="s">
         <v>97</v>
       </c>
       <c r="O106" s="10"/>
@@ -4167,24 +4180,24 @@
       <c r="D108" s="10"/>
       <c r="E108" s="10"/>
       <c r="F108" s="10"/>
-      <c r="G108" s="41" t="s">
+      <c r="G108" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="H108" s="41"/>
-      <c r="I108" s="41"/>
-      <c r="J108" s="41"/>
+      <c r="H108" s="46"/>
+      <c r="I108" s="46"/>
+      <c r="J108" s="46"/>
       <c r="K108" s="10"/>
       <c r="L108" s="10"/>
       <c r="M108" s="10"/>
       <c r="N108" s="10"/>
-      <c r="O108" s="41" t="s">
+      <c r="O108" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="P108" s="41"/>
-      <c r="Q108" s="67" t="s">
+      <c r="P108" s="46"/>
+      <c r="Q108" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="R108" s="67"/>
+      <c r="R108" s="45"/>
       <c r="S108" s="12"/>
     </row>
     <row r="109" spans="1:19" x14ac:dyDescent="0.2">
@@ -4195,20 +4208,20 @@
         <f t="shared" si="0"/>
         <v>6C0</v>
       </c>
-      <c r="C109" s="41" t="s">
+      <c r="C109" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="D109" s="41"/>
-      <c r="E109" s="68" t="s">
+      <c r="D109" s="46"/>
+      <c r="E109" s="47" t="s">
         <v>100</v>
       </c>
-      <c r="F109" s="68"/>
+      <c r="F109" s="47"/>
       <c r="G109" s="10"/>
       <c r="H109" s="10"/>
-      <c r="I109" s="69" t="s">
+      <c r="I109" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="J109" s="70" t="s">
+      <c r="J109" s="38" t="s">
         <v>102</v>
       </c>
       <c r="K109" s="10"/>
@@ -4265,32 +4278,32 @@
         <f t="shared" si="0"/>
         <v>6E0</v>
       </c>
-      <c r="C111" s="44" t="s">
+      <c r="C111" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="D111" s="44"/>
-      <c r="E111" s="44"/>
-      <c r="F111" s="44"/>
+      <c r="D111" s="49"/>
+      <c r="E111" s="49"/>
+      <c r="F111" s="49"/>
       <c r="G111" s="10"/>
       <c r="H111" s="10"/>
       <c r="I111" s="10"/>
       <c r="J111" s="10"/>
-      <c r="K111" s="53" t="s">
+      <c r="K111" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="L111" s="44"/>
-      <c r="M111" s="71" t="s">
+      <c r="L111" s="49"/>
+      <c r="M111" s="48" t="s">
         <v>103</v>
       </c>
-      <c r="N111" s="71"/>
-      <c r="O111" s="44" t="s">
+      <c r="N111" s="48"/>
+      <c r="O111" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="P111" s="44"/>
-      <c r="Q111" s="71" t="s">
+      <c r="P111" s="49"/>
+      <c r="Q111" s="48" t="s">
         <v>105</v>
       </c>
-      <c r="R111" s="71"/>
+      <c r="R111" s="48"/>
       <c r="S111" s="12"/>
     </row>
     <row r="112" spans="1:19" x14ac:dyDescent="0.2">
@@ -4303,10 +4316,10 @@
       </c>
       <c r="C112" s="10"/>
       <c r="D112" s="10"/>
-      <c r="E112" s="72" t="s">
+      <c r="E112" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="F112" s="73" t="s">
+      <c r="F112" s="40" t="s">
         <v>108</v>
       </c>
       <c r="G112" s="10"/>
@@ -4349,12 +4362,12 @@
       <c r="L113" s="10"/>
       <c r="M113" s="10"/>
       <c r="N113" s="10"/>
-      <c r="O113" s="50" t="s">
+      <c r="O113" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="P113" s="50"/>
-      <c r="Q113" s="50"/>
-      <c r="R113" s="50"/>
+      <c r="P113" s="42"/>
+      <c r="Q113" s="42"/>
+      <c r="R113" s="42"/>
       <c r="S113" s="12"/>
     </row>
     <row r="114" spans="1:19" x14ac:dyDescent="0.2">
@@ -4369,28 +4382,28 @@
       <c r="D114" s="10"/>
       <c r="E114" s="10"/>
       <c r="F114" s="10"/>
-      <c r="G114" s="74" t="s">
+      <c r="G114" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="H114" s="74"/>
-      <c r="I114" s="61" t="s">
+      <c r="H114" s="43"/>
+      <c r="I114" s="44" t="s">
         <v>98</v>
       </c>
-      <c r="J114" s="61"/>
-      <c r="K114" s="50" t="s">
+      <c r="J114" s="44"/>
+      <c r="K114" s="42" t="s">
         <v>99</v>
       </c>
-      <c r="L114" s="50"/>
-      <c r="M114" s="61" t="s">
+      <c r="L114" s="42"/>
+      <c r="M114" s="44" t="s">
         <v>100</v>
       </c>
-      <c r="N114" s="61"/>
+      <c r="N114" s="44"/>
       <c r="O114" s="10"/>
       <c r="P114" s="10"/>
-      <c r="Q114" s="75" t="s">
+      <c r="Q114" s="41" t="s">
         <v>101</v>
       </c>
-      <c r="R114" s="49" t="s">
+      <c r="R114" s="28" t="s">
         <v>102</v>
       </c>
       <c r="S114" s="12"/>
@@ -4623,10 +4636,10 @@
       <c r="L123" s="10"/>
       <c r="M123" s="10"/>
       <c r="N123" s="10"/>
-      <c r="O123" s="34"/>
-      <c r="P123" s="27"/>
-      <c r="Q123" s="27"/>
-      <c r="R123" s="27"/>
+      <c r="O123" s="70"/>
+      <c r="P123" s="61"/>
+      <c r="Q123" s="61"/>
+      <c r="R123" s="61"/>
       <c r="S123" s="12" t="s">
         <v>106</v>
       </c>
@@ -4639,22 +4652,22 @@
         <f t="shared" si="0"/>
         <v>7B0</v>
       </c>
-      <c r="C124" s="34"/>
-      <c r="D124" s="27"/>
-      <c r="E124" s="27"/>
-      <c r="F124" s="27"/>
-      <c r="G124" s="27"/>
-      <c r="H124" s="27"/>
-      <c r="I124" s="27"/>
-      <c r="J124" s="27"/>
-      <c r="K124" s="27"/>
-      <c r="L124" s="27"/>
-      <c r="M124" s="27"/>
-      <c r="N124" s="27"/>
-      <c r="O124" s="27"/>
-      <c r="P124" s="27"/>
-      <c r="Q124" s="27"/>
-      <c r="R124" s="27"/>
+      <c r="C124" s="70"/>
+      <c r="D124" s="61"/>
+      <c r="E124" s="61"/>
+      <c r="F124" s="61"/>
+      <c r="G124" s="61"/>
+      <c r="H124" s="61"/>
+      <c r="I124" s="61"/>
+      <c r="J124" s="61"/>
+      <c r="K124" s="61"/>
+      <c r="L124" s="61"/>
+      <c r="M124" s="61"/>
+      <c r="N124" s="61"/>
+      <c r="O124" s="61"/>
+      <c r="P124" s="61"/>
+      <c r="Q124" s="61"/>
+      <c r="R124" s="61"/>
       <c r="S124" s="12"/>
     </row>
     <row r="125" spans="1:19" x14ac:dyDescent="0.2">
@@ -4665,22 +4678,22 @@
         <f t="shared" si="0"/>
         <v>7C0</v>
       </c>
-      <c r="C125" s="27"/>
-      <c r="D125" s="27"/>
-      <c r="E125" s="27"/>
-      <c r="F125" s="27"/>
-      <c r="G125" s="27"/>
-      <c r="H125" s="27"/>
-      <c r="I125" s="27"/>
-      <c r="J125" s="27"/>
-      <c r="K125" s="27"/>
-      <c r="L125" s="27"/>
-      <c r="M125" s="27"/>
-      <c r="N125" s="27"/>
-      <c r="O125" s="27"/>
-      <c r="P125" s="27"/>
-      <c r="Q125" s="27"/>
-      <c r="R125" s="27"/>
+      <c r="C125" s="61"/>
+      <c r="D125" s="61"/>
+      <c r="E125" s="61"/>
+      <c r="F125" s="61"/>
+      <c r="G125" s="61"/>
+      <c r="H125" s="61"/>
+      <c r="I125" s="61"/>
+      <c r="J125" s="61"/>
+      <c r="K125" s="61"/>
+      <c r="L125" s="61"/>
+      <c r="M125" s="61"/>
+      <c r="N125" s="61"/>
+      <c r="O125" s="61"/>
+      <c r="P125" s="61"/>
+      <c r="Q125" s="61"/>
+      <c r="R125" s="61"/>
       <c r="S125" s="12"/>
     </row>
     <row r="126" spans="1:19" x14ac:dyDescent="0.2">
@@ -4691,22 +4704,22 @@
         <f t="shared" si="0"/>
         <v>7D0</v>
       </c>
-      <c r="C126" s="27"/>
-      <c r="D126" s="27"/>
-      <c r="E126" s="27"/>
-      <c r="F126" s="27"/>
-      <c r="G126" s="27"/>
-      <c r="H126" s="27"/>
-      <c r="I126" s="27"/>
-      <c r="J126" s="27"/>
-      <c r="K126" s="27"/>
-      <c r="L126" s="27"/>
-      <c r="M126" s="27"/>
-      <c r="N126" s="27"/>
-      <c r="O126" s="27"/>
-      <c r="P126" s="27"/>
-      <c r="Q126" s="27"/>
-      <c r="R126" s="27"/>
+      <c r="C126" s="61"/>
+      <c r="D126" s="61"/>
+      <c r="E126" s="61"/>
+      <c r="F126" s="61"/>
+      <c r="G126" s="61"/>
+      <c r="H126" s="61"/>
+      <c r="I126" s="61"/>
+      <c r="J126" s="61"/>
+      <c r="K126" s="61"/>
+      <c r="L126" s="61"/>
+      <c r="M126" s="61"/>
+      <c r="N126" s="61"/>
+      <c r="O126" s="61"/>
+      <c r="P126" s="61"/>
+      <c r="Q126" s="61"/>
+      <c r="R126" s="61"/>
       <c r="S126" s="12"/>
     </row>
     <row r="127" spans="1:19" x14ac:dyDescent="0.2">
@@ -4717,22 +4730,22 @@
         <f t="shared" si="0"/>
         <v>7E0</v>
       </c>
-      <c r="C127" s="27"/>
-      <c r="D127" s="27"/>
-      <c r="E127" s="27"/>
-      <c r="F127" s="27"/>
-      <c r="G127" s="27"/>
-      <c r="H127" s="27"/>
-      <c r="I127" s="27"/>
-      <c r="J127" s="27"/>
-      <c r="K127" s="27"/>
-      <c r="L127" s="27"/>
-      <c r="M127" s="27"/>
-      <c r="N127" s="27"/>
-      <c r="O127" s="27"/>
-      <c r="P127" s="27"/>
-      <c r="Q127" s="27"/>
-      <c r="R127" s="27"/>
+      <c r="C127" s="61"/>
+      <c r="D127" s="61"/>
+      <c r="E127" s="61"/>
+      <c r="F127" s="61"/>
+      <c r="G127" s="61"/>
+      <c r="H127" s="61"/>
+      <c r="I127" s="61"/>
+      <c r="J127" s="61"/>
+      <c r="K127" s="61"/>
+      <c r="L127" s="61"/>
+      <c r="M127" s="61"/>
+      <c r="N127" s="61"/>
+      <c r="O127" s="61"/>
+      <c r="P127" s="61"/>
+      <c r="Q127" s="61"/>
+      <c r="R127" s="61"/>
       <c r="S127" s="12"/>
     </row>
     <row r="128" spans="1:19" x14ac:dyDescent="0.2">
@@ -4743,22 +4756,22 @@
         <f t="shared" si="0"/>
         <v>7F0</v>
       </c>
-      <c r="C128" s="27"/>
-      <c r="D128" s="27"/>
-      <c r="E128" s="27"/>
-      <c r="F128" s="27"/>
-      <c r="G128" s="27"/>
-      <c r="H128" s="27"/>
-      <c r="I128" s="27"/>
-      <c r="J128" s="27"/>
-      <c r="K128" s="27"/>
-      <c r="L128" s="27"/>
-      <c r="M128" s="27"/>
-      <c r="N128" s="27"/>
-      <c r="O128" s="27"/>
-      <c r="P128" s="27"/>
-      <c r="Q128" s="27"/>
-      <c r="R128" s="27"/>
+      <c r="C128" s="61"/>
+      <c r="D128" s="61"/>
+      <c r="E128" s="61"/>
+      <c r="F128" s="61"/>
+      <c r="G128" s="61"/>
+      <c r="H128" s="61"/>
+      <c r="I128" s="61"/>
+      <c r="J128" s="61"/>
+      <c r="K128" s="61"/>
+      <c r="L128" s="61"/>
+      <c r="M128" s="61"/>
+      <c r="N128" s="61"/>
+      <c r="O128" s="61"/>
+      <c r="P128" s="61"/>
+      <c r="Q128" s="61"/>
+      <c r="R128" s="61"/>
       <c r="S128" s="12"/>
     </row>
     <row r="129" spans="1:19" x14ac:dyDescent="0.2">
@@ -14955,54 +14968,20 @@
     </row>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="O113:R113"/>
-    <mergeCell ref="G114:H114"/>
-    <mergeCell ref="I114:J114"/>
-    <mergeCell ref="K114:L114"/>
-    <mergeCell ref="M114:N114"/>
-    <mergeCell ref="Q108:R108"/>
-    <mergeCell ref="C109:D109"/>
-    <mergeCell ref="E109:F109"/>
-    <mergeCell ref="M111:N111"/>
-    <mergeCell ref="O111:P111"/>
-    <mergeCell ref="Q111:R111"/>
-    <mergeCell ref="I103:J103"/>
-    <mergeCell ref="K103:L103"/>
-    <mergeCell ref="M103:N103"/>
-    <mergeCell ref="E106:F106"/>
-    <mergeCell ref="G106:H106"/>
-    <mergeCell ref="I106:J106"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="E98:F98"/>
-    <mergeCell ref="M100:N100"/>
-    <mergeCell ref="O100:P100"/>
-    <mergeCell ref="Q100:R100"/>
-    <mergeCell ref="C111:F111"/>
-    <mergeCell ref="O91:R91"/>
-    <mergeCell ref="C106:D106"/>
-    <mergeCell ref="G103:H103"/>
-    <mergeCell ref="O108:P108"/>
-    <mergeCell ref="O97:P97"/>
-    <mergeCell ref="K100:L100"/>
-    <mergeCell ref="K111:L111"/>
-    <mergeCell ref="K94:N94"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="E95:F95"/>
-    <mergeCell ref="G95:H95"/>
-    <mergeCell ref="I95:J95"/>
-    <mergeCell ref="Q97:R97"/>
-    <mergeCell ref="C2:M2"/>
-    <mergeCell ref="N2:R2"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="I3:R3"/>
-    <mergeCell ref="K33:N33"/>
-    <mergeCell ref="O33:R33"/>
-    <mergeCell ref="C72:R86"/>
-    <mergeCell ref="C87:J87"/>
-    <mergeCell ref="L87:R87"/>
-    <mergeCell ref="C88:R88"/>
-    <mergeCell ref="C89:K89"/>
-    <mergeCell ref="L89:R89"/>
+    <mergeCell ref="G50:J50"/>
+    <mergeCell ref="C51:F51"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="K71:R71"/>
+    <mergeCell ref="O34:R34"/>
+    <mergeCell ref="C34:F34"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="K49:N49"/>
+    <mergeCell ref="O49:R49"/>
+    <mergeCell ref="C50:F50"/>
+    <mergeCell ref="O50:R50"/>
+    <mergeCell ref="K35:N35"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="K34:L34"/>
     <mergeCell ref="C90:R90"/>
     <mergeCell ref="O123:R123"/>
     <mergeCell ref="C124:R128"/>
@@ -15017,20 +14996,54 @@
     <mergeCell ref="G97:J97"/>
     <mergeCell ref="O102:R102"/>
     <mergeCell ref="K105:N105"/>
-    <mergeCell ref="G50:J50"/>
-    <mergeCell ref="C51:F51"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="K71:R71"/>
-    <mergeCell ref="O34:R34"/>
-    <mergeCell ref="C34:F34"/>
-    <mergeCell ref="C35:F35"/>
-    <mergeCell ref="K49:N49"/>
-    <mergeCell ref="O49:R49"/>
-    <mergeCell ref="C50:F50"/>
-    <mergeCell ref="O50:R50"/>
-    <mergeCell ref="K35:N35"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="C72:R86"/>
+    <mergeCell ref="C87:J87"/>
+    <mergeCell ref="L87:R87"/>
+    <mergeCell ref="C88:R88"/>
+    <mergeCell ref="C89:K89"/>
+    <mergeCell ref="L89:R89"/>
+    <mergeCell ref="C2:M2"/>
+    <mergeCell ref="N2:R2"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="I3:R3"/>
+    <mergeCell ref="K33:N33"/>
+    <mergeCell ref="O33:R33"/>
+    <mergeCell ref="O91:R91"/>
+    <mergeCell ref="C106:D106"/>
+    <mergeCell ref="G103:H103"/>
+    <mergeCell ref="O108:P108"/>
+    <mergeCell ref="O97:P97"/>
+    <mergeCell ref="K100:L100"/>
+    <mergeCell ref="K94:N94"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="E95:F95"/>
+    <mergeCell ref="G95:H95"/>
+    <mergeCell ref="I95:J95"/>
+    <mergeCell ref="Q97:R97"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="E98:F98"/>
+    <mergeCell ref="M100:N100"/>
+    <mergeCell ref="O100:P100"/>
+    <mergeCell ref="Q100:R100"/>
+    <mergeCell ref="I103:J103"/>
+    <mergeCell ref="K103:L103"/>
+    <mergeCell ref="M103:N103"/>
+    <mergeCell ref="E106:F106"/>
+    <mergeCell ref="G106:H106"/>
+    <mergeCell ref="I106:J106"/>
+    <mergeCell ref="Q108:R108"/>
+    <mergeCell ref="C109:D109"/>
+    <mergeCell ref="E109:F109"/>
+    <mergeCell ref="M111:N111"/>
+    <mergeCell ref="O111:P111"/>
+    <mergeCell ref="Q111:R111"/>
+    <mergeCell ref="C111:F111"/>
+    <mergeCell ref="K111:L111"/>
+    <mergeCell ref="O113:R113"/>
+    <mergeCell ref="G114:H114"/>
+    <mergeCell ref="I114:J114"/>
+    <mergeCell ref="K114:L114"/>
+    <mergeCell ref="M114:N114"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>